<commit_message>
MAP: 100% done, TODO new sectors
</commit_message>
<xml_diff>
--- a/new_universe.xlsx
+++ b/new_universe.xlsx
@@ -24,7 +24,348 @@
     <author>IVAN VUK</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="W2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+S
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+S</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+old map Avarice
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+S
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+E</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+Entry to solar system</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,33 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,349 +415,6 @@
           </rPr>
           <t xml:space="preserve">
 S</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-S
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-Entry to solar system EAST and SOUTH
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-Entry to solar system</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-old map Avarice
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-S
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-E</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-Entry to solar system
-</t>
         </r>
       </text>
     </comment>
@@ -712,59 +684,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-S
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>IVAN VUK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-S</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="J6" authorId="0">
       <text>
         <r>
@@ -945,7 +864,35 @@
             <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-Install pirate base here!</t>
+Entry to solar system
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+Entry to solar system EAST and SOUTH
+</t>
         </r>
       </text>
     </comment>
@@ -2657,6 +2604,33 @@
           </rPr>
           <t xml:space="preserve">
 E
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>IVAN VUK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+S
 </t>
         </r>
       </text>
@@ -7984,9 +7958,6 @@
     <t>Zyarth's Dominion Cluster</t>
   </si>
   <si>
-    <t>Rhea</t>
-  </si>
-  <si>
     <t>11,16</t>
   </si>
   <si>
@@ -8228,6 +8199,9 @@
   </si>
   <si>
     <t>4,13</t>
+  </si>
+  <si>
+    <t>Queen's Harbour Cluster</t>
   </si>
 </sst>
 </file>
@@ -8575,7 +8549,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8828,6 +8802,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="2" xfId="5" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9145,7 +9122,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" thickTop="1" thickBottom="1"/>
@@ -9237,11 +9214,11 @@
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>218</v>
+      <c r="B2" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>267</v>
       </c>
       <c r="R2" s="21" t="s">
         <v>293</v>
@@ -9249,10 +9226,10 @@
       <c r="S2" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="25" t="s">
         <v>239</v>
       </c>
     </row>
@@ -9260,11 +9237,11 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>214</v>
+      <c r="B3" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>266</v>
       </c>
       <c r="R3" s="33" t="s">
         <v>142</v>
@@ -9272,10 +9249,10 @@
       <c r="S3" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="88" t="s">
         <v>241</v>
       </c>
     </row>
@@ -9283,29 +9260,26 @@
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>215</v>
+      <c r="B4" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>269</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>231</v>
-      </c>
       <c r="I4" s="4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>134</v>
@@ -9328,13 +9302,13 @@
       <c r="T4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="U4" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="28" t="s">
         <v>242</v>
       </c>
     </row>
@@ -9342,8 +9316,8 @@
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>252</v>
+      <c r="B5" s="23" t="s">
+        <v>316</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>14</v>
@@ -9352,16 +9326,16 @@
         <v>175</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>166</v>
@@ -9393,13 +9367,13 @@
       <c r="T5" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="U5" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="25" t="s">
         <v>244</v>
       </c>
     </row>
@@ -9414,16 +9388,16 @@
         <v>71</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>165</v>
@@ -9464,10 +9438,10 @@
       <c r="U6" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="W6" s="39" t="s">
         <v>245</v>
       </c>
     </row>
@@ -9485,10 +9459,10 @@
         <v>75</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>567</v>
+        <v>252</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>26</v>
@@ -9534,9 +9508,6 @@
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>483</v>
-      </c>
       <c r="D8" s="26" t="s">
         <v>114</v>
       </c>
@@ -9590,9 +9561,6 @@
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>316</v>
-      </c>
       <c r="D9" s="26" t="s">
         <v>115</v>
       </c>
@@ -10052,6 +10020,9 @@
       <c r="P16" s="23" t="s">
         <v>318</v>
       </c>
+      <c r="Q16" s="4" t="s">
+        <v>227</v>
+      </c>
       <c r="R16" s="25" t="s">
         <v>103</v>
       </c>
@@ -10213,11 +10184,11 @@
       <c r="O19" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="P19" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q19" s="18" t="s">
-        <v>267</v>
+      <c r="P19" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="R19" s="39" t="s">
         <v>28</v>
@@ -10263,11 +10234,11 @@
       <c r="O20" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="P20" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q20" s="18" t="s">
-        <v>266</v>
+      <c r="P20" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="R20" s="39" t="s">
         <v>36</v>
@@ -10301,8 +10272,11 @@
       <c r="O21" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="Q21" s="18" t="s">
-        <v>269</v>
+      <c r="P21" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="R21" s="39" t="s">
         <v>43</v>
@@ -10321,7 +10295,7 @@
       </c>
       <c r="C23" s="6">
         <f>COUNTA(B2:Y21)</f>
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="42" customHeight="1" thickTop="1" thickBot="1">
@@ -10330,7 +10304,7 @@
       </c>
       <c r="C24" s="6">
         <f>COUNTBLANK(B2:Y21)</f>
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" ht="42" customHeight="1"/>
@@ -11384,8 +11358,8 @@
   <dimension ref="A1:I513"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E239" sqref="E239"/>
+      <pane ySplit="2" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A238" sqref="A238:XFD238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15187,13 +15161,13 @@
     </row>
     <row r="188" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A188" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B188" s="37" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C188" s="37" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D188" t="s">
         <v>325</v>
@@ -15205,7 +15179,7 @@
         <v>325</v>
       </c>
       <c r="H188" s="48" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I188" s="48"/>
     </row>
@@ -15214,10 +15188,10 @@
         <v>67</v>
       </c>
       <c r="B189" s="37" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C189" s="37" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D189" t="s">
         <v>325</v>
@@ -15236,7 +15210,7 @@
         <v>173</v>
       </c>
       <c r="B190" s="37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C190" s="37" t="s">
         <v>451</v>
@@ -15258,10 +15232,10 @@
         <v>68</v>
       </c>
       <c r="B191" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C191" s="37" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D191" t="s">
         <v>325</v>
@@ -15280,10 +15254,10 @@
         <v>172</v>
       </c>
       <c r="B192" s="37" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C192" s="37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D192" t="s">
         <v>325</v>
@@ -15302,10 +15276,10 @@
         <v>171</v>
       </c>
       <c r="B193" s="37" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C193" s="37" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D193" t="s">
         <v>325</v>
@@ -15327,7 +15301,7 @@
         <v>410</v>
       </c>
       <c r="C194" s="37" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D194" t="s">
         <v>325</v>
@@ -15353,7 +15327,7 @@
         <v>437</v>
       </c>
       <c r="C196" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D196" t="s">
         <v>325</v>
@@ -15365,7 +15339,7 @@
         <v>325</v>
       </c>
       <c r="H196" s="49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I196" s="49"/>
     </row>
@@ -15374,10 +15348,10 @@
         <v>190</v>
       </c>
       <c r="B197" s="37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C197" s="37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D197" t="s">
         <v>325</v>
@@ -15396,10 +15370,10 @@
         <v>191</v>
       </c>
       <c r="B198" s="37" t="s">
+        <v>584</v>
+      </c>
+      <c r="C198" s="37" t="s">
         <v>585</v>
-      </c>
-      <c r="C198" s="37" t="s">
-        <v>586</v>
       </c>
       <c r="D198" t="s">
         <v>325</v>
@@ -15418,10 +15392,10 @@
         <v>192</v>
       </c>
       <c r="B199" s="37" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C199" s="37" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D199" t="s">
         <v>325</v>
@@ -15444,10 +15418,10 @@
         <v>187</v>
       </c>
       <c r="B201" s="37" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C201" s="37" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D201" t="s">
         <v>325</v>
@@ -15459,7 +15433,7 @@
         <v>325</v>
       </c>
       <c r="H201" s="50" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I201" s="50"/>
     </row>
@@ -15493,7 +15467,7 @@
         <v>385</v>
       </c>
       <c r="C203" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D203" t="s">
         <v>325</v>
@@ -15515,7 +15489,7 @@
         <v>387</v>
       </c>
       <c r="C204" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D204" t="s">
         <v>325</v>
@@ -15534,10 +15508,10 @@
         <v>156</v>
       </c>
       <c r="B205" s="37" t="s">
+        <v>593</v>
+      </c>
+      <c r="C205" s="37" t="s">
         <v>594</v>
-      </c>
-      <c r="C205" s="37" t="s">
-        <v>595</v>
       </c>
       <c r="D205" t="s">
         <v>325</v>
@@ -15556,10 +15530,10 @@
         <v>157</v>
       </c>
       <c r="B206" s="37" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C206" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D206" t="s">
         <v>325</v>
@@ -15579,14 +15553,14 @@
     </row>
     <row r="208" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A208" t="s">
+        <v>609</v>
+      </c>
+      <c r="B208" s="37" t="s">
+        <v>611</v>
+      </c>
+      <c r="C208" s="37" t="s">
         <v>610</v>
       </c>
-      <c r="B208" s="37" t="s">
-        <v>612</v>
-      </c>
-      <c r="C208" s="37" t="s">
-        <v>611</v>
-      </c>
       <c r="D208" t="s">
         <v>325</v>
       </c>
@@ -15597,7 +15571,7 @@
         <v>325</v>
       </c>
       <c r="H208" s="51" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I208" s="51"/>
     </row>
@@ -15606,10 +15580,10 @@
         <v>3</v>
       </c>
       <c r="B209" s="37" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C209" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D209" t="s">
         <v>325</v>
@@ -15625,13 +15599,13 @@
     </row>
     <row r="210" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A210" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B210" s="37" t="s">
         <v>414</v>
       </c>
       <c r="C210" s="37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D210" t="s">
         <v>325</v>
@@ -15650,10 +15624,10 @@
         <v>79</v>
       </c>
       <c r="B211" s="37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C211" s="37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D211" t="s">
         <v>325</v>
@@ -15672,10 +15646,10 @@
         <v>4</v>
       </c>
       <c r="B212" s="37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C212" s="37" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D212" t="s">
         <v>325</v>
@@ -15713,7 +15687,7 @@
         <v>325</v>
       </c>
       <c r="H214" s="52" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I214" s="52"/>
     </row>
@@ -15722,10 +15696,10 @@
         <v>21</v>
       </c>
       <c r="B215" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C215" s="37" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D215" t="s">
         <v>325</v>
@@ -15747,7 +15721,7 @@
         <v>371</v>
       </c>
       <c r="C216" s="37" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D216" t="s">
         <v>325</v>
@@ -15766,7 +15740,7 @@
         <v>119</v>
       </c>
       <c r="B217" s="37" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C217" s="37" t="s">
         <v>350</v>
@@ -15788,10 +15762,10 @@
         <v>29</v>
       </c>
       <c r="B218" s="37" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C218" s="37" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D218" t="s">
         <v>325</v>
@@ -15807,13 +15781,13 @@
     </row>
     <row r="219" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A219" t="s">
+        <v>626</v>
+      </c>
+      <c r="B219" s="37" t="s">
+        <v>628</v>
+      </c>
+      <c r="C219" s="37" t="s">
         <v>627</v>
-      </c>
-      <c r="B219" s="37" t="s">
-        <v>629</v>
-      </c>
-      <c r="C219" s="37" t="s">
-        <v>628</v>
       </c>
       <c r="D219" t="s">
         <v>325</v>
@@ -15832,10 +15806,10 @@
         <v>37</v>
       </c>
       <c r="B220" s="37" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C220" s="37" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D220" t="s">
         <v>325</v>
@@ -15854,10 +15828,10 @@
         <v>85</v>
       </c>
       <c r="B221" s="37" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C221" s="37" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D221" t="s">
         <v>325</v>
@@ -15876,10 +15850,10 @@
         <v>44</v>
       </c>
       <c r="B222" s="37" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C222" s="37" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D222" t="s">
         <v>325</v>
@@ -15898,10 +15872,10 @@
         <v>186</v>
       </c>
       <c r="B223" s="37" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C223" s="37" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D223" t="s">
         <v>325</v>
@@ -15915,11 +15889,11 @@
       <c r="H223" s="52"/>
       <c r="I223" s="52"/>
     </row>
-    <row r="224" spans="1:9" s="24" customFormat="1" ht="15" thickTop="1">
+    <row r="224" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B224" s="38"/>
       <c r="C224" s="38"/>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A225" t="s">
         <v>202</v>
       </c>
@@ -15935,13 +15909,17 @@
       <c r="E225" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="226" spans="1:5">
+      <c r="H225" s="51" t="s">
+        <v>648</v>
+      </c>
+      <c r="I225" s="51"/>
+    </row>
+    <row r="226" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A226" t="s">
         <v>203</v>
       </c>
       <c r="B226" s="37" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C226" s="37" t="s">
         <v>411</v>
@@ -15952,8 +15930,10 @@
       <c r="E226" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="227" spans="1:5">
+      <c r="H226" s="51"/>
+      <c r="I226" s="51"/>
+    </row>
+    <row r="227" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A227" t="s">
         <v>129</v>
       </c>
@@ -15961,7 +15941,7 @@
         <v>367</v>
       </c>
       <c r="C227" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D227" t="s">
         <v>325</v>
@@ -15969,8 +15949,10 @@
       <c r="E227" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="228" spans="1:5">
+      <c r="H227" s="51"/>
+      <c r="I227" s="51"/>
+    </row>
+    <row r="228" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A228" t="s">
         <v>123</v>
       </c>
@@ -15978,7 +15960,7 @@
         <v>345</v>
       </c>
       <c r="C228" s="37" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D228" t="s">
         <v>325</v>
@@ -15986,8 +15968,10 @@
       <c r="E228" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="229" spans="1:5">
+      <c r="H228" s="51"/>
+      <c r="I228" s="51"/>
+    </row>
+    <row r="229" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A229" t="s">
         <v>207</v>
       </c>
@@ -15995,7 +15979,7 @@
         <v>493</v>
       </c>
       <c r="C229" s="37" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D229" t="s">
         <v>325</v>
@@ -16003,16 +15987,18 @@
       <c r="E229" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="230" spans="1:5">
+      <c r="H229" s="51"/>
+      <c r="I229" s="51"/>
+    </row>
+    <row r="230" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A230" t="s">
         <v>204</v>
       </c>
       <c r="B230" s="37" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C230" s="37" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D230" t="s">
         <v>325</v>
@@ -16020,8 +16006,10 @@
       <c r="E230" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="231" spans="1:5">
+      <c r="H230" s="51"/>
+      <c r="I230" s="51"/>
+    </row>
+    <row r="231" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A231" t="s">
         <v>205</v>
       </c>
@@ -16037,16 +16025,18 @@
       <c r="E231" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="232" spans="1:5">
+      <c r="H231" s="51"/>
+      <c r="I231" s="51"/>
+    </row>
+    <row r="232" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A232" t="s">
         <v>152</v>
       </c>
       <c r="B232" s="37" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C232" s="37" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D232" t="s">
         <v>325</v>
@@ -16054,16 +16044,18 @@
       <c r="E232" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="233" spans="1:5">
+      <c r="H232" s="51"/>
+      <c r="I232" s="51"/>
+    </row>
+    <row r="233" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A233" t="s">
         <v>121</v>
       </c>
       <c r="B233" s="37" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C233" s="37" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D233" t="s">
         <v>325</v>
@@ -16071,8 +16063,10 @@
       <c r="E233" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="234" spans="1:5">
+      <c r="H233" s="51"/>
+      <c r="I233" s="51"/>
+    </row>
+    <row r="234" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A234" t="s">
         <v>208</v>
       </c>
@@ -16088,8 +16082,10 @@
       <c r="E234" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="235" spans="1:5">
+      <c r="H234" s="51"/>
+      <c r="I234" s="51"/>
+    </row>
+    <row r="235" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A235" t="s">
         <v>122</v>
       </c>
@@ -16105,8 +16101,10 @@
       <c r="E235" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="236" spans="1:5">
+      <c r="H235" s="51"/>
+      <c r="I235" s="51"/>
+    </row>
+    <row r="236" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A236" t="s">
         <v>206</v>
       </c>
@@ -16122,8 +16120,10 @@
       <c r="E236" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="237" spans="1:5">
+      <c r="H236" s="51"/>
+      <c r="I236" s="51"/>
+    </row>
+    <row r="237" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A237" t="s">
         <v>128</v>
       </c>
@@ -16131,7 +16131,7 @@
         <v>369</v>
       </c>
       <c r="C237" s="37" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D237" t="s">
         <v>325</v>
@@ -16139,16 +16139,18 @@
       <c r="E237" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="238" spans="1:5">
-      <c r="B238" s="37"/>
-      <c r="C238" s="37"/>
-    </row>
-    <row r="239" spans="1:5">
+      <c r="H237" s="51"/>
+      <c r="I237" s="51"/>
+    </row>
+    <row r="238" spans="1:9" s="24" customFormat="1" ht="15" thickTop="1">
+      <c r="B238" s="38"/>
+      <c r="C238" s="38"/>
+    </row>
+    <row r="239" spans="1:9">
       <c r="B239" s="37"/>
       <c r="C239" s="37"/>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:9">
       <c r="B240" s="37"/>
       <c r="C240" s="37"/>
     </row>
@@ -17244,7 +17246,8 @@
       <c r="C513" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="H225:I237"/>
     <mergeCell ref="H149:I158"/>
     <mergeCell ref="H160:I166"/>
     <mergeCell ref="H168:I170"/>
@@ -17284,8 +17287,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" thickTop="1" thickBottom="1"/>
@@ -17622,42 +17625,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B1" t="s">
         <v>599</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>600</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>601</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F1" t="s">
         <v>602</v>
-      </c>
-      <c r="E1" t="s">
-        <v>604</v>
-      </c>
-      <c r="F1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B2" t="s">
+        <v>604</v>
+      </c>
+      <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>606</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>607</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>608</v>
-      </c>
-      <c r="F2" t="s">
-        <v>609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MOV: fix, wrong file version
</commit_message>
<xml_diff>
--- a/new_universe.xlsx
+++ b/new_universe.xlsx
@@ -8555,58 +8555,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="4">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="7">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="2" xfId="6">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="12" borderId="2" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="2" xfId="12">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1">
@@ -8693,7 +8651,49 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="7">
+    <xf numFmtId="49" fontId="1" fillId="12" borderId="2" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="2" xfId="12">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="2" xfId="6">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9008,10 +9008,10 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" thickTop="1" thickBottom="1"/>
@@ -11318,10 +11318,10 @@
       <c r="G3" t="s">
         <v>324</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="I3" s="68"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A4" t="s">
@@ -11342,8 +11342,8 @@
       <c r="G4" t="s">
         <v>324</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A5" t="s">
@@ -11364,8 +11364,8 @@
       <c r="G5" t="s">
         <v>324</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A6" t="s">
@@ -11386,8 +11386,8 @@
       <c r="G6" t="s">
         <v>324</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A7" t="s">
@@ -11408,8 +11408,8 @@
       <c r="G7" t="s">
         <v>324</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A8" t="s">
@@ -11430,8 +11430,8 @@
       <c r="G8" t="s">
         <v>324</v>
       </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A9" t="s">
@@ -11452,8 +11452,8 @@
       <c r="G9" t="s">
         <v>324</v>
       </c>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A10" t="s">
@@ -11474,8 +11474,8 @@
       <c r="G10" t="s">
         <v>324</v>
       </c>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11" t="s">
@@ -11496,8 +11496,8 @@
       <c r="G11" t="s">
         <v>324</v>
       </c>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12" t="s">
@@ -11518,8 +11518,8 @@
       <c r="G12" t="s">
         <v>324</v>
       </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" t="s">
@@ -11540,8 +11540,8 @@
       <c r="G13" t="s">
         <v>324</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
     </row>
     <row r="14" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B14" s="38"/>
@@ -11566,10 +11566,10 @@
       <c r="G15" t="s">
         <v>324</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="54" t="s">
         <v>331</v>
       </c>
-      <c r="I15" s="57"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A16" t="s">
@@ -11590,8 +11590,8 @@
       <c r="G16" t="s">
         <v>324</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
     </row>
     <row r="17" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A17" t="s">
@@ -11612,8 +11612,8 @@
       <c r="G17" t="s">
         <v>324</v>
       </c>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A18" t="s">
@@ -11634,8 +11634,8 @@
       <c r="G18" t="s">
         <v>324</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A19" t="s">
@@ -11656,8 +11656,8 @@
       <c r="G19" t="s">
         <v>324</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A20" t="s">
@@ -11678,8 +11678,8 @@
       <c r="G20" t="s">
         <v>324</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A21" t="s">
@@ -11700,8 +11700,8 @@
       <c r="G21" t="s">
         <v>324</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A22" t="s">
@@ -11722,8 +11722,8 @@
       <c r="G22" t="s">
         <v>324</v>
       </c>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A23" t="s">
@@ -11744,8 +11744,8 @@
       <c r="G23" t="s">
         <v>324</v>
       </c>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B24" s="38"/>
@@ -11770,10 +11770,10 @@
       <c r="G25" t="s">
         <v>324</v>
       </c>
-      <c r="H25" s="69" t="s">
+      <c r="H25" s="55" t="s">
         <v>334</v>
       </c>
-      <c r="I25" s="69"/>
+      <c r="I25" s="55"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A26" t="s">
@@ -11794,8 +11794,8 @@
       <c r="G26" t="s">
         <v>324</v>
       </c>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
     </row>
     <row r="27" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A27" t="s">
@@ -11816,8 +11816,8 @@
       <c r="G27" t="s">
         <v>324</v>
       </c>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
     </row>
     <row r="28" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A28" t="s">
@@ -11838,8 +11838,8 @@
       <c r="G28" t="s">
         <v>324</v>
       </c>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
     </row>
     <row r="29" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A29" t="s">
@@ -11860,8 +11860,8 @@
       <c r="G29" t="s">
         <v>324</v>
       </c>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A30" t="s">
@@ -11882,8 +11882,8 @@
       <c r="G30" t="s">
         <v>324</v>
       </c>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A31" t="s">
@@ -11904,8 +11904,8 @@
       <c r="G31" t="s">
         <v>324</v>
       </c>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
     </row>
     <row r="32" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B32" s="38"/>
@@ -11930,10 +11930,10 @@
       <c r="G33" t="s">
         <v>324</v>
       </c>
-      <c r="H33" s="70" t="s">
+      <c r="H33" s="56" t="s">
         <v>336</v>
       </c>
-      <c r="I33" s="70"/>
+      <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
@@ -11954,8 +11954,8 @@
       <c r="G34" t="s">
         <v>324</v>
       </c>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
@@ -11976,8 +11976,8 @@
       <c r="G35" t="s">
         <v>324</v>
       </c>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
@@ -11998,8 +11998,8 @@
       <c r="G36" t="s">
         <v>324</v>
       </c>
-      <c r="H36" s="71"/>
-      <c r="I36" s="71"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
@@ -12020,8 +12020,8 @@
       <c r="G37" t="s">
         <v>324</v>
       </c>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
@@ -12042,8 +12042,8 @@
       <c r="G38" t="s">
         <v>324</v>
       </c>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
@@ -12064,8 +12064,8 @@
       <c r="G39" t="s">
         <v>324</v>
       </c>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
@@ -12086,8 +12086,8 @@
       <c r="G40" t="s">
         <v>324</v>
       </c>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
@@ -12108,8 +12108,8 @@
       <c r="G41" t="s">
         <v>324</v>
       </c>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
@@ -12130,8 +12130,8 @@
       <c r="G42" t="s">
         <v>324</v>
       </c>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B43" s="38"/>
@@ -12158,10 +12158,10 @@
       <c r="G44" t="s">
         <v>324</v>
       </c>
-      <c r="H44" s="69" t="s">
+      <c r="H44" s="55" t="s">
         <v>338</v>
       </c>
-      <c r="I44" s="69"/>
+      <c r="I44" s="55"/>
     </row>
     <row r="45" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A45" t="s">
@@ -12182,8 +12182,8 @@
       <c r="G45" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
     </row>
     <row r="46" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A46" t="s">
@@ -12204,8 +12204,8 @@
       <c r="G46" t="s">
         <v>324</v>
       </c>
-      <c r="H46" s="69"/>
-      <c r="I46" s="69"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
     </row>
     <row r="47" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A47" t="s">
@@ -12226,8 +12226,8 @@
       <c r="G47" t="s">
         <v>324</v>
       </c>
-      <c r="H47" s="69"/>
-      <c r="I47" s="69"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
     </row>
     <row r="48" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" t="s">
@@ -12248,8 +12248,8 @@
       <c r="G48" t="s">
         <v>324</v>
       </c>
-      <c r="H48" s="69"/>
-      <c r="I48" s="69"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
     </row>
     <row r="49" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A49" t="s">
@@ -12270,8 +12270,8 @@
       <c r="G49" t="s">
         <v>324</v>
       </c>
-      <c r="H49" s="69"/>
-      <c r="I49" s="69"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="55"/>
     </row>
     <row r="50" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B50" s="38"/>
@@ -12296,10 +12296,10 @@
       <c r="G51" t="s">
         <v>324</v>
       </c>
-      <c r="H51" s="79" t="s">
+      <c r="H51" s="65" t="s">
         <v>339</v>
       </c>
-      <c r="I51" s="80"/>
+      <c r="I51" s="66"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
@@ -12320,8 +12320,8 @@
       <c r="G52" t="s">
         <v>324</v>
       </c>
-      <c r="H52" s="81"/>
-      <c r="I52" s="82"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="68"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
@@ -12342,8 +12342,8 @@
       <c r="G53" t="s">
         <v>324</v>
       </c>
-      <c r="H53" s="81"/>
-      <c r="I53" s="82"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="68"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
@@ -12364,8 +12364,8 @@
       <c r="G54" t="s">
         <v>324</v>
       </c>
-      <c r="H54" s="81"/>
-      <c r="I54" s="82"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="68"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
@@ -12386,8 +12386,8 @@
       <c r="G55" t="s">
         <v>324</v>
       </c>
-      <c r="H55" s="81"/>
-      <c r="I55" s="82"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="68"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
@@ -12408,8 +12408,8 @@
       <c r="G56" t="s">
         <v>324</v>
       </c>
-      <c r="H56" s="81"/>
-      <c r="I56" s="82"/>
+      <c r="H56" s="67"/>
+      <c r="I56" s="68"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
@@ -12430,8 +12430,8 @@
       <c r="G57" t="s">
         <v>324</v>
       </c>
-      <c r="H57" s="81"/>
-      <c r="I57" s="82"/>
+      <c r="H57" s="67"/>
+      <c r="I57" s="68"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
@@ -12452,8 +12452,8 @@
       <c r="G58" t="s">
         <v>324</v>
       </c>
-      <c r="H58" s="81"/>
-      <c r="I58" s="82"/>
+      <c r="H58" s="67"/>
+      <c r="I58" s="68"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -12474,8 +12474,8 @@
       <c r="G59" t="s">
         <v>324</v>
       </c>
-      <c r="H59" s="81"/>
-      <c r="I59" s="82"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="68"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
@@ -12496,8 +12496,8 @@
       <c r="G60" t="s">
         <v>324</v>
       </c>
-      <c r="H60" s="81"/>
-      <c r="I60" s="82"/>
+      <c r="H60" s="67"/>
+      <c r="I60" s="68"/>
     </row>
     <row r="61" spans="1:9" ht="15" thickBot="1">
       <c r="A61" t="s">
@@ -12515,8 +12515,8 @@
       <c r="E61" t="s">
         <v>324</v>
       </c>
-      <c r="H61" s="83"/>
-      <c r="I61" s="84"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="70"/>
     </row>
     <row r="62" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B62" s="38"/>
@@ -12541,10 +12541,10 @@
       <c r="G63" t="s">
         <v>324</v>
       </c>
-      <c r="H63" s="57" t="s">
+      <c r="H63" s="54" t="s">
         <v>350</v>
       </c>
-      <c r="I63" s="57"/>
+      <c r="I63" s="54"/>
     </row>
     <row r="64" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A64" t="s">
@@ -12565,8 +12565,8 @@
       <c r="G64" t="s">
         <v>324</v>
       </c>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
+      <c r="H64" s="54"/>
+      <c r="I64" s="54"/>
     </row>
     <row r="65" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A65" t="s">
@@ -12587,8 +12587,8 @@
       <c r="G65" t="s">
         <v>324</v>
       </c>
-      <c r="H65" s="57"/>
-      <c r="I65" s="57"/>
+      <c r="H65" s="54"/>
+      <c r="I65" s="54"/>
     </row>
     <row r="66" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A66" t="s">
@@ -12609,8 +12609,8 @@
       <c r="G66" t="s">
         <v>324</v>
       </c>
-      <c r="H66" s="57"/>
-      <c r="I66" s="57"/>
+      <c r="H66" s="54"/>
+      <c r="I66" s="54"/>
     </row>
     <row r="67" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A67" t="s">
@@ -12631,8 +12631,8 @@
       <c r="G67" t="s">
         <v>324</v>
       </c>
-      <c r="H67" s="57"/>
-      <c r="I67" s="57"/>
+      <c r="H67" s="54"/>
+      <c r="I67" s="54"/>
     </row>
     <row r="68" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B68" s="38"/>
@@ -12657,10 +12657,10 @@
       <c r="G69" t="s">
         <v>324</v>
       </c>
-      <c r="H69" s="76" t="s">
+      <c r="H69" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="I69" s="76"/>
+      <c r="I69" s="62"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
@@ -12681,8 +12681,8 @@
       <c r="G70" t="s">
         <v>324</v>
       </c>
-      <c r="H70" s="77"/>
-      <c r="I70" s="77"/>
+      <c r="H70" s="63"/>
+      <c r="I70" s="63"/>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
@@ -12703,8 +12703,8 @@
       <c r="G71" t="s">
         <v>324</v>
       </c>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
+      <c r="H71" s="63"/>
+      <c r="I71" s="63"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
@@ -12725,8 +12725,8 @@
       <c r="G72" t="s">
         <v>324</v>
       </c>
-      <c r="H72" s="77"/>
-      <c r="I72" s="77"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
@@ -12747,8 +12747,8 @@
       <c r="G73" t="s">
         <v>324</v>
       </c>
-      <c r="H73" s="77"/>
-      <c r="I73" s="77"/>
+      <c r="H73" s="63"/>
+      <c r="I73" s="63"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
@@ -12769,8 +12769,8 @@
       <c r="G74" t="s">
         <v>324</v>
       </c>
-      <c r="H74" s="77"/>
-      <c r="I74" s="77"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="63"/>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
@@ -12791,8 +12791,8 @@
       <c r="G75" t="s">
         <v>324</v>
       </c>
-      <c r="H75" s="77"/>
-      <c r="I75" s="77"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
@@ -12813,8 +12813,8 @@
       <c r="G76" t="s">
         <v>324</v>
       </c>
-      <c r="H76" s="77"/>
-      <c r="I76" s="77"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="63"/>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
@@ -12835,8 +12835,8 @@
       <c r="G77" t="s">
         <v>324</v>
       </c>
-      <c r="H77" s="77"/>
-      <c r="I77" s="77"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="63"/>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
@@ -12857,8 +12857,8 @@
       <c r="G78" t="s">
         <v>324</v>
       </c>
-      <c r="H78" s="78"/>
-      <c r="I78" s="78"/>
+      <c r="H78" s="64"/>
+      <c r="I78" s="64"/>
     </row>
     <row r="79" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B79" s="38"/>
@@ -12883,10 +12883,10 @@
       <c r="G80" t="s">
         <v>324</v>
       </c>
-      <c r="H80" s="85" t="s">
+      <c r="H80" s="71" t="s">
         <v>406</v>
       </c>
-      <c r="I80" s="86"/>
+      <c r="I80" s="72"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
@@ -12907,8 +12907,8 @@
       <c r="G81" t="s">
         <v>324</v>
       </c>
-      <c r="H81" s="87"/>
-      <c r="I81" s="88"/>
+      <c r="H81" s="73"/>
+      <c r="I81" s="74"/>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
@@ -12929,8 +12929,8 @@
       <c r="G82" t="s">
         <v>324</v>
       </c>
-      <c r="H82" s="87"/>
-      <c r="I82" s="88"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="74"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
@@ -12951,8 +12951,8 @@
       <c r="G83" t="s">
         <v>324</v>
       </c>
-      <c r="H83" s="87"/>
-      <c r="I83" s="88"/>
+      <c r="H83" s="73"/>
+      <c r="I83" s="74"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
@@ -12973,8 +12973,8 @@
       <c r="G84" t="s">
         <v>324</v>
       </c>
-      <c r="H84" s="87"/>
-      <c r="I84" s="88"/>
+      <c r="H84" s="73"/>
+      <c r="I84" s="74"/>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
@@ -12995,8 +12995,8 @@
       <c r="G85" t="s">
         <v>324</v>
       </c>
-      <c r="H85" s="87"/>
-      <c r="I85" s="88"/>
+      <c r="H85" s="73"/>
+      <c r="I85" s="74"/>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
@@ -13017,8 +13017,8 @@
       <c r="G86" t="s">
         <v>324</v>
       </c>
-      <c r="H86" s="87"/>
-      <c r="I86" s="88"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="74"/>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
@@ -13039,8 +13039,8 @@
       <c r="G87" t="s">
         <v>324</v>
       </c>
-      <c r="H87" s="87"/>
-      <c r="I87" s="88"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="74"/>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
@@ -13061,8 +13061,8 @@
       <c r="G88" t="s">
         <v>324</v>
       </c>
-      <c r="H88" s="87"/>
-      <c r="I88" s="88"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="74"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
@@ -13083,8 +13083,8 @@
       <c r="G89" t="s">
         <v>324</v>
       </c>
-      <c r="H89" s="87"/>
-      <c r="I89" s="88"/>
+      <c r="H89" s="73"/>
+      <c r="I89" s="74"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
@@ -13105,8 +13105,8 @@
       <c r="G90" t="s">
         <v>324</v>
       </c>
-      <c r="H90" s="87"/>
-      <c r="I90" s="88"/>
+      <c r="H90" s="73"/>
+      <c r="I90" s="74"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
@@ -13127,8 +13127,8 @@
       <c r="G91" t="s">
         <v>324</v>
       </c>
-      <c r="H91" s="87"/>
-      <c r="I91" s="88"/>
+      <c r="H91" s="73"/>
+      <c r="I91" s="74"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
@@ -13149,8 +13149,8 @@
       <c r="G92" t="s">
         <v>324</v>
       </c>
-      <c r="H92" s="87"/>
-      <c r="I92" s="88"/>
+      <c r="H92" s="73"/>
+      <c r="I92" s="74"/>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
@@ -13171,8 +13171,8 @@
       <c r="G93" t="s">
         <v>324</v>
       </c>
-      <c r="H93" s="87"/>
-      <c r="I93" s="88"/>
+      <c r="H93" s="73"/>
+      <c r="I93" s="74"/>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
@@ -13193,8 +13193,8 @@
       <c r="G94" t="s">
         <v>324</v>
       </c>
-      <c r="H94" s="87"/>
-      <c r="I94" s="88"/>
+      <c r="H94" s="73"/>
+      <c r="I94" s="74"/>
     </row>
     <row r="95" spans="1:9" ht="15" thickBot="1">
       <c r="A95" t="s">
@@ -13215,8 +13215,8 @@
       <c r="G95" t="s">
         <v>324</v>
       </c>
-      <c r="H95" s="89"/>
-      <c r="I95" s="90"/>
+      <c r="H95" s="75"/>
+      <c r="I95" s="76"/>
     </row>
     <row r="96" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B96" s="38"/>
@@ -13241,10 +13241,10 @@
       <c r="G97" t="s">
         <v>324</v>
       </c>
-      <c r="H97" s="69" t="s">
+      <c r="H97" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="I97" s="69"/>
+      <c r="I97" s="55"/>
     </row>
     <row r="98" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A98" t="s">
@@ -13265,8 +13265,8 @@
       <c r="G98" t="s">
         <v>324</v>
       </c>
-      <c r="H98" s="69"/>
-      <c r="I98" s="69"/>
+      <c r="H98" s="55"/>
+      <c r="I98" s="55"/>
     </row>
     <row r="99" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A99" t="s">
@@ -13287,8 +13287,8 @@
       <c r="G99" t="s">
         <v>324</v>
       </c>
-      <c r="H99" s="69"/>
-      <c r="I99" s="69"/>
+      <c r="H99" s="55"/>
+      <c r="I99" s="55"/>
     </row>
     <row r="100" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A100" t="s">
@@ -13309,8 +13309,8 @@
       <c r="G100" t="s">
         <v>324</v>
       </c>
-      <c r="H100" s="69"/>
-      <c r="I100" s="69"/>
+      <c r="H100" s="55"/>
+      <c r="I100" s="55"/>
     </row>
     <row r="101" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A101" t="s">
@@ -13331,8 +13331,8 @@
       <c r="G101" t="s">
         <v>324</v>
       </c>
-      <c r="H101" s="69"/>
-      <c r="I101" s="69"/>
+      <c r="H101" s="55"/>
+      <c r="I101" s="55"/>
     </row>
     <row r="102" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A102" t="s">
@@ -13353,8 +13353,8 @@
       <c r="G102" t="s">
         <v>324</v>
       </c>
-      <c r="H102" s="69"/>
-      <c r="I102" s="69"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="55"/>
     </row>
     <row r="103" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B103" s="38"/>
@@ -13379,10 +13379,10 @@
       <c r="G104" t="s">
         <v>324</v>
       </c>
-      <c r="H104" s="79" t="s">
+      <c r="H104" s="65" t="s">
         <v>428</v>
       </c>
-      <c r="I104" s="80"/>
+      <c r="I104" s="66"/>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
@@ -13403,8 +13403,8 @@
       <c r="G105" t="s">
         <v>324</v>
       </c>
-      <c r="H105" s="81"/>
-      <c r="I105" s="82"/>
+      <c r="H105" s="67"/>
+      <c r="I105" s="68"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
@@ -13425,8 +13425,8 @@
       <c r="G106" t="s">
         <v>324</v>
       </c>
-      <c r="H106" s="81"/>
-      <c r="I106" s="82"/>
+      <c r="H106" s="67"/>
+      <c r="I106" s="68"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
@@ -13447,8 +13447,8 @@
       <c r="G107" t="s">
         <v>324</v>
       </c>
-      <c r="H107" s="81"/>
-      <c r="I107" s="82"/>
+      <c r="H107" s="67"/>
+      <c r="I107" s="68"/>
     </row>
     <row r="108" spans="1:9" ht="15" thickBot="1">
       <c r="A108" t="s">
@@ -13469,8 +13469,8 @@
       <c r="G108" t="s">
         <v>324</v>
       </c>
-      <c r="H108" s="83"/>
-      <c r="I108" s="84"/>
+      <c r="H108" s="69"/>
+      <c r="I108" s="70"/>
     </row>
     <row r="109" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B109" s="38"/>
@@ -13495,10 +13495,10 @@
       <c r="G110" t="s">
         <v>324</v>
       </c>
-      <c r="H110" s="91" t="s">
+      <c r="H110" s="77" t="s">
         <v>448</v>
       </c>
-      <c r="I110" s="92"/>
+      <c r="I110" s="78"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
@@ -13519,8 +13519,8 @@
       <c r="G111" t="s">
         <v>324</v>
       </c>
-      <c r="H111" s="93"/>
-      <c r="I111" s="94"/>
+      <c r="H111" s="79"/>
+      <c r="I111" s="80"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
@@ -13541,8 +13541,8 @@
       <c r="G112" t="s">
         <v>324</v>
       </c>
-      <c r="H112" s="93"/>
-      <c r="I112" s="94"/>
+      <c r="H112" s="79"/>
+      <c r="I112" s="80"/>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
@@ -13563,8 +13563,8 @@
       <c r="G113" t="s">
         <v>324</v>
       </c>
-      <c r="H113" s="93"/>
-      <c r="I113" s="94"/>
+      <c r="H113" s="79"/>
+      <c r="I113" s="80"/>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
@@ -13585,8 +13585,8 @@
       <c r="G114" t="s">
         <v>324</v>
       </c>
-      <c r="H114" s="93"/>
-      <c r="I114" s="94"/>
+      <c r="H114" s="79"/>
+      <c r="I114" s="80"/>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
@@ -13607,8 +13607,8 @@
       <c r="G115" t="s">
         <v>324</v>
       </c>
-      <c r="H115" s="93"/>
-      <c r="I115" s="94"/>
+      <c r="H115" s="79"/>
+      <c r="I115" s="80"/>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
@@ -13629,8 +13629,8 @@
       <c r="G116" t="s">
         <v>324</v>
       </c>
-      <c r="H116" s="93"/>
-      <c r="I116" s="94"/>
+      <c r="H116" s="79"/>
+      <c r="I116" s="80"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
@@ -13651,8 +13651,8 @@
       <c r="G117" t="s">
         <v>324</v>
       </c>
-      <c r="H117" s="93"/>
-      <c r="I117" s="94"/>
+      <c r="H117" s="79"/>
+      <c r="I117" s="80"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
@@ -13673,8 +13673,8 @@
       <c r="G118" t="s">
         <v>324</v>
       </c>
-      <c r="H118" s="93"/>
-      <c r="I118" s="94"/>
+      <c r="H118" s="79"/>
+      <c r="I118" s="80"/>
     </row>
     <row r="119" spans="1:9" ht="15" thickBot="1">
       <c r="A119" t="s">
@@ -13695,8 +13695,8 @@
       <c r="G119" t="s">
         <v>324</v>
       </c>
-      <c r="H119" s="95"/>
-      <c r="I119" s="96"/>
+      <c r="H119" s="81"/>
+      <c r="I119" s="82"/>
     </row>
     <row r="120" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B120" s="38"/>
@@ -13721,10 +13721,10 @@
       <c r="G121" t="s">
         <v>324</v>
       </c>
-      <c r="H121" s="79" t="s">
+      <c r="H121" s="65" t="s">
         <v>463</v>
       </c>
-      <c r="I121" s="80"/>
+      <c r="I121" s="66"/>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
@@ -13745,8 +13745,8 @@
       <c r="G122" t="s">
         <v>324</v>
       </c>
-      <c r="H122" s="81"/>
-      <c r="I122" s="82"/>
+      <c r="H122" s="67"/>
+      <c r="I122" s="68"/>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
@@ -13767,8 +13767,8 @@
       <c r="G123" t="s">
         <v>324</v>
       </c>
-      <c r="H123" s="81"/>
-      <c r="I123" s="82"/>
+      <c r="H123" s="67"/>
+      <c r="I123" s="68"/>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
@@ -13789,8 +13789,8 @@
       <c r="G124" t="s">
         <v>324</v>
       </c>
-      <c r="H124" s="81"/>
-      <c r="I124" s="82"/>
+      <c r="H124" s="67"/>
+      <c r="I124" s="68"/>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
@@ -13811,8 +13811,8 @@
       <c r="G125" t="s">
         <v>324</v>
       </c>
-      <c r="H125" s="81"/>
-      <c r="I125" s="82"/>
+      <c r="H125" s="67"/>
+      <c r="I125" s="68"/>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
@@ -13833,8 +13833,8 @@
       <c r="G126" t="s">
         <v>324</v>
       </c>
-      <c r="H126" s="81"/>
-      <c r="I126" s="82"/>
+      <c r="H126" s="67"/>
+      <c r="I126" s="68"/>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
@@ -13855,8 +13855,8 @@
       <c r="G127" t="s">
         <v>324</v>
       </c>
-      <c r="H127" s="81"/>
-      <c r="I127" s="82"/>
+      <c r="H127" s="67"/>
+      <c r="I127" s="68"/>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
@@ -13877,8 +13877,8 @@
       <c r="G128" t="s">
         <v>324</v>
       </c>
-      <c r="H128" s="81"/>
-      <c r="I128" s="82"/>
+      <c r="H128" s="67"/>
+      <c r="I128" s="68"/>
     </row>
     <row r="129" spans="1:9" ht="15" thickBot="1">
       <c r="A129" t="s">
@@ -13899,8 +13899,8 @@
       <c r="G129" t="s">
         <v>324</v>
       </c>
-      <c r="H129" s="83"/>
-      <c r="I129" s="84"/>
+      <c r="H129" s="69"/>
+      <c r="I129" s="70"/>
     </row>
     <row r="130" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B130" s="38"/>
@@ -13925,10 +13925,10 @@
       <c r="G131" t="s">
         <v>324</v>
       </c>
-      <c r="H131" s="69" t="s">
+      <c r="H131" s="55" t="s">
         <v>479</v>
       </c>
-      <c r="I131" s="69"/>
+      <c r="I131" s="55"/>
     </row>
     <row r="132" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A132" t="s">
@@ -13949,8 +13949,8 @@
       <c r="G132" t="s">
         <v>324</v>
       </c>
-      <c r="H132" s="69"/>
-      <c r="I132" s="69"/>
+      <c r="H132" s="55"/>
+      <c r="I132" s="55"/>
     </row>
     <row r="133" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A133" t="s">
@@ -13971,8 +13971,8 @@
       <c r="G133" t="s">
         <v>324</v>
       </c>
-      <c r="H133" s="69"/>
-      <c r="I133" s="69"/>
+      <c r="H133" s="55"/>
+      <c r="I133" s="55"/>
     </row>
     <row r="134" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A134" t="s">
@@ -13993,8 +13993,8 @@
       <c r="G134" t="s">
         <v>324</v>
       </c>
-      <c r="H134" s="69"/>
-      <c r="I134" s="69"/>
+      <c r="H134" s="55"/>
+      <c r="I134" s="55"/>
     </row>
     <row r="135" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A135" t="s">
@@ -14015,8 +14015,8 @@
       <c r="G135" t="s">
         <v>324</v>
       </c>
-      <c r="H135" s="69"/>
-      <c r="I135" s="69"/>
+      <c r="H135" s="55"/>
+      <c r="I135" s="55"/>
     </row>
     <row r="136" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A136" t="s">
@@ -14037,8 +14037,8 @@
       <c r="G136" t="s">
         <v>324</v>
       </c>
-      <c r="H136" s="69"/>
-      <c r="I136" s="69"/>
+      <c r="H136" s="55"/>
+      <c r="I136" s="55"/>
     </row>
     <row r="137" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A137" t="s">
@@ -14059,8 +14059,8 @@
       <c r="G137" t="s">
         <v>324</v>
       </c>
-      <c r="H137" s="69"/>
-      <c r="I137" s="69"/>
+      <c r="H137" s="55"/>
+      <c r="I137" s="55"/>
     </row>
     <row r="138" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A138" t="s">
@@ -14081,8 +14081,8 @@
       <c r="G138" t="s">
         <v>324</v>
       </c>
-      <c r="H138" s="69"/>
-      <c r="I138" s="69"/>
+      <c r="H138" s="55"/>
+      <c r="I138" s="55"/>
     </row>
     <row r="139" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B139" s="38"/>
@@ -14107,10 +14107,10 @@
       <c r="G140" t="s">
         <v>324</v>
       </c>
-      <c r="H140" s="73" t="s">
+      <c r="H140" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="I140" s="73"/>
+      <c r="I140" s="59"/>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" t="s">
@@ -14131,8 +14131,8 @@
       <c r="G141" t="s">
         <v>324</v>
       </c>
-      <c r="H141" s="74"/>
-      <c r="I141" s="74"/>
+      <c r="H141" s="60"/>
+      <c r="I141" s="60"/>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" t="s">
@@ -14153,8 +14153,8 @@
       <c r="G142" t="s">
         <v>324</v>
       </c>
-      <c r="H142" s="74"/>
-      <c r="I142" s="74"/>
+      <c r="H142" s="60"/>
+      <c r="I142" s="60"/>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" t="s">
@@ -14175,8 +14175,8 @@
       <c r="G143" t="s">
         <v>324</v>
       </c>
-      <c r="H143" s="74"/>
-      <c r="I143" s="74"/>
+      <c r="H143" s="60"/>
+      <c r="I143" s="60"/>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="41" t="s">
@@ -14197,8 +14197,8 @@
       <c r="G144" t="s">
         <v>324</v>
       </c>
-      <c r="H144" s="74"/>
-      <c r="I144" s="74"/>
+      <c r="H144" s="60"/>
+      <c r="I144" s="60"/>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" t="s">
@@ -14219,8 +14219,8 @@
       <c r="G145" t="s">
         <v>324</v>
       </c>
-      <c r="H145" s="74"/>
-      <c r="I145" s="74"/>
+      <c r="H145" s="60"/>
+      <c r="I145" s="60"/>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" t="s">
@@ -14241,8 +14241,8 @@
       <c r="G146" t="s">
         <v>324</v>
       </c>
-      <c r="H146" s="74"/>
-      <c r="I146" s="74"/>
+      <c r="H146" s="60"/>
+      <c r="I146" s="60"/>
     </row>
     <row r="147" spans="1:9">
       <c r="A147" t="s">
@@ -14263,8 +14263,8 @@
       <c r="G147" t="s">
         <v>324</v>
       </c>
-      <c r="H147" s="75"/>
-      <c r="I147" s="75"/>
+      <c r="H147" s="61"/>
+      <c r="I147" s="61"/>
     </row>
     <row r="148" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B148" s="38"/>
@@ -14289,10 +14289,10 @@
       <c r="G149" t="s">
         <v>324</v>
       </c>
-      <c r="H149" s="59" t="s">
+      <c r="H149" s="51" t="s">
         <v>518</v>
       </c>
-      <c r="I149" s="59"/>
+      <c r="I149" s="51"/>
     </row>
     <row r="150" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A150" t="s">
@@ -14313,8 +14313,8 @@
       <c r="G150" t="s">
         <v>324</v>
       </c>
-      <c r="H150" s="59"/>
-      <c r="I150" s="59"/>
+      <c r="H150" s="51"/>
+      <c r="I150" s="51"/>
     </row>
     <row r="151" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A151" t="s">
@@ -14335,8 +14335,8 @@
       <c r="G151" t="s">
         <v>324</v>
       </c>
-      <c r="H151" s="59"/>
-      <c r="I151" s="59"/>
+      <c r="H151" s="51"/>
+      <c r="I151" s="51"/>
     </row>
     <row r="152" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A152" t="s">
@@ -14357,8 +14357,8 @@
       <c r="G152" t="s">
         <v>324</v>
       </c>
-      <c r="H152" s="59"/>
-      <c r="I152" s="59"/>
+      <c r="H152" s="51"/>
+      <c r="I152" s="51"/>
     </row>
     <row r="153" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A153" t="s">
@@ -14379,8 +14379,8 @@
       <c r="G153" t="s">
         <v>324</v>
       </c>
-      <c r="H153" s="59"/>
-      <c r="I153" s="59"/>
+      <c r="H153" s="51"/>
+      <c r="I153" s="51"/>
     </row>
     <row r="154" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A154" t="s">
@@ -14401,8 +14401,8 @@
       <c r="G154" t="s">
         <v>324</v>
       </c>
-      <c r="H154" s="59"/>
-      <c r="I154" s="59"/>
+      <c r="H154" s="51"/>
+      <c r="I154" s="51"/>
     </row>
     <row r="155" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A155" t="s">
@@ -14423,8 +14423,8 @@
       <c r="G155" t="s">
         <v>324</v>
       </c>
-      <c r="H155" s="59"/>
-      <c r="I155" s="59"/>
+      <c r="H155" s="51"/>
+      <c r="I155" s="51"/>
     </row>
     <row r="156" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A156" t="s">
@@ -14445,8 +14445,8 @@
       <c r="G156" t="s">
         <v>324</v>
       </c>
-      <c r="H156" s="59"/>
-      <c r="I156" s="59"/>
+      <c r="H156" s="51"/>
+      <c r="I156" s="51"/>
     </row>
     <row r="157" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A157" t="s">
@@ -14467,8 +14467,8 @@
       <c r="G157" t="s">
         <v>324</v>
       </c>
-      <c r="H157" s="59"/>
-      <c r="I157" s="59"/>
+      <c r="H157" s="51"/>
+      <c r="I157" s="51"/>
     </row>
     <row r="158" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A158" t="s">
@@ -14489,8 +14489,8 @@
       <c r="G158" t="s">
         <v>324</v>
       </c>
-      <c r="H158" s="59"/>
-      <c r="I158" s="59"/>
+      <c r="H158" s="51"/>
+      <c r="I158" s="51"/>
     </row>
     <row r="159" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B159" s="38"/>
@@ -14515,10 +14515,10 @@
       <c r="G160" t="s">
         <v>324</v>
       </c>
-      <c r="H160" s="60" t="s">
+      <c r="H160" s="83" t="s">
         <v>532</v>
       </c>
-      <c r="I160" s="60"/>
+      <c r="I160" s="83"/>
     </row>
     <row r="161" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A161" t="s">
@@ -14539,8 +14539,8 @@
       <c r="G161" t="s">
         <v>324</v>
       </c>
-      <c r="H161" s="60"/>
-      <c r="I161" s="60"/>
+      <c r="H161" s="83"/>
+      <c r="I161" s="83"/>
     </row>
     <row r="162" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A162" t="s">
@@ -14561,8 +14561,8 @@
       <c r="G162" t="s">
         <v>324</v>
       </c>
-      <c r="H162" s="60"/>
-      <c r="I162" s="60"/>
+      <c r="H162" s="83"/>
+      <c r="I162" s="83"/>
     </row>
     <row r="163" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A163" t="s">
@@ -14583,8 +14583,8 @@
       <c r="G163" t="s">
         <v>324</v>
       </c>
-      <c r="H163" s="60"/>
-      <c r="I163" s="60"/>
+      <c r="H163" s="83"/>
+      <c r="I163" s="83"/>
     </row>
     <row r="164" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A164" t="s">
@@ -14605,8 +14605,8 @@
       <c r="G164" t="s">
         <v>324</v>
       </c>
-      <c r="H164" s="60"/>
-      <c r="I164" s="60"/>
+      <c r="H164" s="83"/>
+      <c r="I164" s="83"/>
     </row>
     <row r="165" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A165" t="s">
@@ -14627,8 +14627,8 @@
       <c r="G165" t="s">
         <v>324</v>
       </c>
-      <c r="H165" s="60"/>
-      <c r="I165" s="60"/>
+      <c r="H165" s="83"/>
+      <c r="I165" s="83"/>
     </row>
     <row r="166" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A166" t="s">
@@ -14649,8 +14649,8 @@
       <c r="G166" t="s">
         <v>324</v>
       </c>
-      <c r="H166" s="60"/>
-      <c r="I166" s="60"/>
+      <c r="H166" s="83"/>
+      <c r="I166" s="83"/>
     </row>
     <row r="167" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B167" s="38"/>
@@ -14675,10 +14675,10 @@
       <c r="G168" t="s">
         <v>324</v>
       </c>
-      <c r="H168" s="61" t="s">
+      <c r="H168" s="84" t="s">
         <v>540</v>
       </c>
-      <c r="I168" s="61"/>
+      <c r="I168" s="84"/>
     </row>
     <row r="169" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A169" t="s">
@@ -14699,8 +14699,8 @@
       <c r="G169" t="s">
         <v>324</v>
       </c>
-      <c r="H169" s="61"/>
-      <c r="I169" s="61"/>
+      <c r="H169" s="84"/>
+      <c r="I169" s="84"/>
     </row>
     <row r="170" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A170" t="s">
@@ -14721,8 +14721,8 @@
       <c r="G170" t="s">
         <v>324</v>
       </c>
-      <c r="H170" s="61"/>
-      <c r="I170" s="61"/>
+      <c r="H170" s="84"/>
+      <c r="I170" s="84"/>
     </row>
     <row r="171" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B171" s="38"/>
@@ -14747,10 +14747,10 @@
       <c r="G172" t="s">
         <v>324</v>
       </c>
-      <c r="H172" s="57" t="s">
+      <c r="H172" s="54" t="s">
         <v>557</v>
       </c>
-      <c r="I172" s="57"/>
+      <c r="I172" s="54"/>
     </row>
     <row r="173" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A173" t="s">
@@ -14771,8 +14771,8 @@
       <c r="G173" t="s">
         <v>324</v>
       </c>
-      <c r="H173" s="57"/>
-      <c r="I173" s="57"/>
+      <c r="H173" s="54"/>
+      <c r="I173" s="54"/>
     </row>
     <row r="174" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A174" t="s">
@@ -14793,8 +14793,8 @@
       <c r="G174" t="s">
         <v>324</v>
       </c>
-      <c r="H174" s="57"/>
-      <c r="I174" s="57"/>
+      <c r="H174" s="54"/>
+      <c r="I174" s="54"/>
     </row>
     <row r="175" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A175" t="s">
@@ -14815,8 +14815,8 @@
       <c r="G175" t="s">
         <v>324</v>
       </c>
-      <c r="H175" s="57"/>
-      <c r="I175" s="57"/>
+      <c r="H175" s="54"/>
+      <c r="I175" s="54"/>
     </row>
     <row r="176" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A176" t="s">
@@ -14837,8 +14837,8 @@
       <c r="G176" t="s">
         <v>324</v>
       </c>
-      <c r="H176" s="57"/>
-      <c r="I176" s="57"/>
+      <c r="H176" s="54"/>
+      <c r="I176" s="54"/>
     </row>
     <row r="177" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A177" t="s">
@@ -14859,8 +14859,8 @@
       <c r="G177" t="s">
         <v>324</v>
       </c>
-      <c r="H177" s="57"/>
-      <c r="I177" s="57"/>
+      <c r="H177" s="54"/>
+      <c r="I177" s="54"/>
     </row>
     <row r="178" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A178" t="s">
@@ -14881,8 +14881,8 @@
       <c r="G178" t="s">
         <v>324</v>
       </c>
-      <c r="H178" s="57"/>
-      <c r="I178" s="57"/>
+      <c r="H178" s="54"/>
+      <c r="I178" s="54"/>
     </row>
     <row r="179" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A179" s="41" t="s">
@@ -14903,8 +14903,8 @@
       <c r="G179" t="s">
         <v>324</v>
       </c>
-      <c r="H179" s="57"/>
-      <c r="I179" s="57"/>
+      <c r="H179" s="54"/>
+      <c r="I179" s="54"/>
     </row>
     <row r="180" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B180" s="38"/>
@@ -14929,10 +14929,10 @@
       <c r="G181" t="s">
         <v>324</v>
       </c>
-      <c r="H181" s="62" t="s">
+      <c r="H181" s="85" t="s">
         <v>565</v>
       </c>
-      <c r="I181" s="63"/>
+      <c r="I181" s="86"/>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" t="s">
@@ -14953,8 +14953,8 @@
       <c r="G182" t="s">
         <v>324</v>
       </c>
-      <c r="H182" s="64"/>
-      <c r="I182" s="65"/>
+      <c r="H182" s="87"/>
+      <c r="I182" s="88"/>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
@@ -14975,8 +14975,8 @@
       <c r="G183" t="s">
         <v>324</v>
       </c>
-      <c r="H183" s="64"/>
-      <c r="I183" s="65"/>
+      <c r="H183" s="87"/>
+      <c r="I183" s="88"/>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" t="s">
@@ -14997,8 +14997,8 @@
       <c r="G184" t="s">
         <v>324</v>
       </c>
-      <c r="H184" s="64"/>
-      <c r="I184" s="65"/>
+      <c r="H184" s="87"/>
+      <c r="I184" s="88"/>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" t="s">
@@ -15019,8 +15019,8 @@
       <c r="G185" t="s">
         <v>324</v>
       </c>
-      <c r="H185" s="64"/>
-      <c r="I185" s="65"/>
+      <c r="H185" s="87"/>
+      <c r="I185" s="88"/>
     </row>
     <row r="186" spans="1:9" ht="15" thickBot="1">
       <c r="A186" t="s">
@@ -15041,8 +15041,8 @@
       <c r="G186" t="s">
         <v>324</v>
       </c>
-      <c r="H186" s="66"/>
-      <c r="I186" s="67"/>
+      <c r="H186" s="89"/>
+      <c r="I186" s="90"/>
     </row>
     <row r="187" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B187" s="38"/>
@@ -15067,10 +15067,10 @@
       <c r="G188" t="s">
         <v>324</v>
       </c>
-      <c r="H188" s="59" t="s">
+      <c r="H188" s="51" t="s">
         <v>580</v>
       </c>
-      <c r="I188" s="59"/>
+      <c r="I188" s="51"/>
     </row>
     <row r="189" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A189" t="s">
@@ -15091,8 +15091,8 @@
       <c r="G189" t="s">
         <v>324</v>
       </c>
-      <c r="H189" s="59"/>
-      <c r="I189" s="59"/>
+      <c r="H189" s="51"/>
+      <c r="I189" s="51"/>
     </row>
     <row r="190" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A190" t="s">
@@ -15113,8 +15113,8 @@
       <c r="G190" t="s">
         <v>324</v>
       </c>
-      <c r="H190" s="59"/>
-      <c r="I190" s="59"/>
+      <c r="H190" s="51"/>
+      <c r="I190" s="51"/>
     </row>
     <row r="191" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A191" t="s">
@@ -15135,8 +15135,8 @@
       <c r="G191" t="s">
         <v>324</v>
       </c>
-      <c r="H191" s="59"/>
-      <c r="I191" s="59"/>
+      <c r="H191" s="51"/>
+      <c r="I191" s="51"/>
     </row>
     <row r="192" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A192" t="s">
@@ -15157,8 +15157,8 @@
       <c r="G192" t="s">
         <v>324</v>
       </c>
-      <c r="H192" s="59"/>
-      <c r="I192" s="59"/>
+      <c r="H192" s="51"/>
+      <c r="I192" s="51"/>
     </row>
     <row r="193" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A193" t="s">
@@ -15179,8 +15179,8 @@
       <c r="G193" t="s">
         <v>324</v>
       </c>
-      <c r="H193" s="59"/>
-      <c r="I193" s="59"/>
+      <c r="H193" s="51"/>
+      <c r="I193" s="51"/>
     </row>
     <row r="194" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A194" t="s">
@@ -15201,8 +15201,8 @@
       <c r="G194" t="s">
         <v>324</v>
       </c>
-      <c r="H194" s="59"/>
-      <c r="I194" s="59"/>
+      <c r="H194" s="51"/>
+      <c r="I194" s="51"/>
     </row>
     <row r="195" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B195" s="38"/>
@@ -15227,10 +15227,10 @@
       <c r="G196" t="s">
         <v>324</v>
       </c>
-      <c r="H196" s="97" t="s">
+      <c r="H196" s="52" t="s">
         <v>587</v>
       </c>
-      <c r="I196" s="97"/>
+      <c r="I196" s="52"/>
     </row>
     <row r="197" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A197" t="s">
@@ -15251,8 +15251,8 @@
       <c r="G197" t="s">
         <v>324</v>
       </c>
-      <c r="H197" s="97"/>
-      <c r="I197" s="97"/>
+      <c r="H197" s="52"/>
+      <c r="I197" s="52"/>
     </row>
     <row r="198" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A198" t="s">
@@ -15273,8 +15273,8 @@
       <c r="G198" t="s">
         <v>324</v>
       </c>
-      <c r="H198" s="97"/>
-      <c r="I198" s="97"/>
+      <c r="H198" s="52"/>
+      <c r="I198" s="52"/>
     </row>
     <row r="199" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A199" t="s">
@@ -15295,8 +15295,8 @@
       <c r="G199" t="s">
         <v>324</v>
       </c>
-      <c r="H199" s="97"/>
-      <c r="I199" s="97"/>
+      <c r="H199" s="52"/>
+      <c r="I199" s="52"/>
     </row>
     <row r="200" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B200" s="38"/>
@@ -15321,10 +15321,10 @@
       <c r="G201" t="s">
         <v>324</v>
       </c>
-      <c r="H201" s="68" t="s">
+      <c r="H201" s="53" t="s">
         <v>596</v>
       </c>
-      <c r="I201" s="68"/>
+      <c r="I201" s="53"/>
     </row>
     <row r="202" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A202" t="s">
@@ -15345,8 +15345,8 @@
       <c r="G202" t="s">
         <v>324</v>
       </c>
-      <c r="H202" s="68"/>
-      <c r="I202" s="68"/>
+      <c r="H202" s="53"/>
+      <c r="I202" s="53"/>
     </row>
     <row r="203" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A203" t="s">
@@ -15367,8 +15367,8 @@
       <c r="G203" t="s">
         <v>324</v>
       </c>
-      <c r="H203" s="68"/>
-      <c r="I203" s="68"/>
+      <c r="H203" s="53"/>
+      <c r="I203" s="53"/>
     </row>
     <row r="204" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A204" t="s">
@@ -15389,8 +15389,8 @@
       <c r="G204" t="s">
         <v>324</v>
       </c>
-      <c r="H204" s="68"/>
-      <c r="I204" s="68"/>
+      <c r="H204" s="53"/>
+      <c r="I204" s="53"/>
     </row>
     <row r="205" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A205" t="s">
@@ -15411,8 +15411,8 @@
       <c r="G205" t="s">
         <v>324</v>
       </c>
-      <c r="H205" s="68"/>
-      <c r="I205" s="68"/>
+      <c r="H205" s="53"/>
+      <c r="I205" s="53"/>
     </row>
     <row r="206" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A206" t="s">
@@ -15433,8 +15433,8 @@
       <c r="G206" t="s">
         <v>324</v>
       </c>
-      <c r="H206" s="68"/>
-      <c r="I206" s="68"/>
+      <c r="H206" s="53"/>
+      <c r="I206" s="53"/>
     </row>
     <row r="207" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B207" s="38"/>
@@ -15459,10 +15459,10 @@
       <c r="G208" t="s">
         <v>324</v>
       </c>
-      <c r="H208" s="57" t="s">
+      <c r="H208" s="54" t="s">
         <v>619</v>
       </c>
-      <c r="I208" s="57"/>
+      <c r="I208" s="54"/>
     </row>
     <row r="209" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A209" t="s">
@@ -15483,8 +15483,8 @@
       <c r="G209" t="s">
         <v>324</v>
       </c>
-      <c r="H209" s="57"/>
-      <c r="I209" s="57"/>
+      <c r="H209" s="54"/>
+      <c r="I209" s="54"/>
     </row>
     <row r="210" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A210" t="s">
@@ -15505,8 +15505,8 @@
       <c r="G210" t="s">
         <v>324</v>
       </c>
-      <c r="H210" s="57"/>
-      <c r="I210" s="57"/>
+      <c r="H210" s="54"/>
+      <c r="I210" s="54"/>
     </row>
     <row r="211" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A211" t="s">
@@ -15527,8 +15527,8 @@
       <c r="G211" t="s">
         <v>324</v>
       </c>
-      <c r="H211" s="57"/>
-      <c r="I211" s="57"/>
+      <c r="H211" s="54"/>
+      <c r="I211" s="54"/>
     </row>
     <row r="212" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A212" t="s">
@@ -15549,8 +15549,8 @@
       <c r="G212" t="s">
         <v>324</v>
       </c>
-      <c r="H212" s="57"/>
-      <c r="I212" s="57"/>
+      <c r="H212" s="54"/>
+      <c r="I212" s="54"/>
     </row>
     <row r="213" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B213" s="38"/>
@@ -15575,10 +15575,10 @@
       <c r="G214" t="s">
         <v>324</v>
       </c>
-      <c r="H214" s="69" t="s">
+      <c r="H214" s="55" t="s">
         <v>636</v>
       </c>
-      <c r="I214" s="69"/>
+      <c r="I214" s="55"/>
     </row>
     <row r="215" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A215" t="s">
@@ -15599,8 +15599,8 @@
       <c r="G215" t="s">
         <v>324</v>
       </c>
-      <c r="H215" s="69"/>
-      <c r="I215" s="69"/>
+      <c r="H215" s="55"/>
+      <c r="I215" s="55"/>
     </row>
     <row r="216" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A216" t="s">
@@ -15621,8 +15621,8 @@
       <c r="G216" t="s">
         <v>324</v>
       </c>
-      <c r="H216" s="69"/>
-      <c r="I216" s="69"/>
+      <c r="H216" s="55"/>
+      <c r="I216" s="55"/>
     </row>
     <row r="217" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A217" t="s">
@@ -15643,8 +15643,8 @@
       <c r="G217" t="s">
         <v>324</v>
       </c>
-      <c r="H217" s="69"/>
-      <c r="I217" s="69"/>
+      <c r="H217" s="55"/>
+      <c r="I217" s="55"/>
     </row>
     <row r="218" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A218" t="s">
@@ -15665,8 +15665,8 @@
       <c r="G218" t="s">
         <v>324</v>
       </c>
-      <c r="H218" s="69"/>
-      <c r="I218" s="69"/>
+      <c r="H218" s="55"/>
+      <c r="I218" s="55"/>
     </row>
     <row r="219" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A219" t="s">
@@ -15687,8 +15687,8 @@
       <c r="G219" t="s">
         <v>324</v>
       </c>
-      <c r="H219" s="69"/>
-      <c r="I219" s="69"/>
+      <c r="H219" s="55"/>
+      <c r="I219" s="55"/>
     </row>
     <row r="220" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A220" t="s">
@@ -15709,8 +15709,8 @@
       <c r="G220" t="s">
         <v>324</v>
       </c>
-      <c r="H220" s="69"/>
-      <c r="I220" s="69"/>
+      <c r="H220" s="55"/>
+      <c r="I220" s="55"/>
     </row>
     <row r="221" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A221" t="s">
@@ -15731,8 +15731,8 @@
       <c r="G221" t="s">
         <v>324</v>
       </c>
-      <c r="H221" s="69"/>
-      <c r="I221" s="69"/>
+      <c r="H221" s="55"/>
+      <c r="I221" s="55"/>
     </row>
     <row r="222" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A222" t="s">
@@ -15753,8 +15753,8 @@
       <c r="G222" t="s">
         <v>324</v>
       </c>
-      <c r="H222" s="69"/>
-      <c r="I222" s="69"/>
+      <c r="H222" s="55"/>
+      <c r="I222" s="55"/>
     </row>
     <row r="223" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A223" t="s">
@@ -15775,8 +15775,8 @@
       <c r="G223" t="s">
         <v>324</v>
       </c>
-      <c r="H223" s="69"/>
-      <c r="I223" s="69"/>
+      <c r="H223" s="55"/>
+      <c r="I223" s="55"/>
     </row>
     <row r="224" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B224" s="38"/>
@@ -15801,10 +15801,10 @@
       <c r="G225" t="s">
         <v>324</v>
       </c>
-      <c r="H225" s="57" t="s">
+      <c r="H225" s="54" t="s">
         <v>647</v>
       </c>
-      <c r="I225" s="57"/>
+      <c r="I225" s="54"/>
     </row>
     <row r="226" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A226" t="s">
@@ -15825,8 +15825,8 @@
       <c r="G226" t="s">
         <v>324</v>
       </c>
-      <c r="H226" s="57"/>
-      <c r="I226" s="57"/>
+      <c r="H226" s="54"/>
+      <c r="I226" s="54"/>
     </row>
     <row r="227" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A227" t="s">
@@ -15847,8 +15847,8 @@
       <c r="G227" t="s">
         <v>324</v>
       </c>
-      <c r="H227" s="57"/>
-      <c r="I227" s="57"/>
+      <c r="H227" s="54"/>
+      <c r="I227" s="54"/>
     </row>
     <row r="228" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A228" t="s">
@@ -15869,8 +15869,8 @@
       <c r="G228" t="s">
         <v>324</v>
       </c>
-      <c r="H228" s="57"/>
-      <c r="I228" s="57"/>
+      <c r="H228" s="54"/>
+      <c r="I228" s="54"/>
     </row>
     <row r="229" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A229" t="s">
@@ -15891,8 +15891,8 @@
       <c r="G229" t="s">
         <v>324</v>
       </c>
-      <c r="H229" s="57"/>
-      <c r="I229" s="57"/>
+      <c r="H229" s="54"/>
+      <c r="I229" s="54"/>
     </row>
     <row r="230" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A230" t="s">
@@ -15913,8 +15913,8 @@
       <c r="G230" t="s">
         <v>324</v>
       </c>
-      <c r="H230" s="57"/>
-      <c r="I230" s="57"/>
+      <c r="H230" s="54"/>
+      <c r="I230" s="54"/>
     </row>
     <row r="231" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A231" t="s">
@@ -15935,8 +15935,8 @@
       <c r="G231" t="s">
         <v>324</v>
       </c>
-      <c r="H231" s="57"/>
-      <c r="I231" s="57"/>
+      <c r="H231" s="54"/>
+      <c r="I231" s="54"/>
     </row>
     <row r="232" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A232" t="s">
@@ -15957,8 +15957,8 @@
       <c r="G232" t="s">
         <v>324</v>
       </c>
-      <c r="H232" s="57"/>
-      <c r="I232" s="57"/>
+      <c r="H232" s="54"/>
+      <c r="I232" s="54"/>
     </row>
     <row r="233" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A233" t="s">
@@ -15979,8 +15979,8 @@
       <c r="G233" t="s">
         <v>324</v>
       </c>
-      <c r="H233" s="57"/>
-      <c r="I233" s="57"/>
+      <c r="H233" s="54"/>
+      <c r="I233" s="54"/>
     </row>
     <row r="234" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A234" t="s">
@@ -16001,8 +16001,8 @@
       <c r="G234" t="s">
         <v>324</v>
       </c>
-      <c r="H234" s="57"/>
-      <c r="I234" s="57"/>
+      <c r="H234" s="54"/>
+      <c r="I234" s="54"/>
     </row>
     <row r="235" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A235" t="s">
@@ -16023,8 +16023,8 @@
       <c r="G235" t="s">
         <v>324</v>
       </c>
-      <c r="H235" s="57"/>
-      <c r="I235" s="57"/>
+      <c r="H235" s="54"/>
+      <c r="I235" s="54"/>
     </row>
     <row r="236" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A236" t="s">
@@ -16045,8 +16045,8 @@
       <c r="G236" t="s">
         <v>324</v>
       </c>
-      <c r="H236" s="57"/>
-      <c r="I236" s="57"/>
+      <c r="H236" s="54"/>
+      <c r="I236" s="54"/>
     </row>
     <row r="237" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A237" t="s">
@@ -16067,8 +16067,8 @@
       <c r="G237" t="s">
         <v>324</v>
       </c>
-      <c r="H237" s="57"/>
-      <c r="I237" s="57"/>
+      <c r="H237" s="54"/>
+      <c r="I237" s="54"/>
     </row>
     <row r="238" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B238" s="38"/>
@@ -16090,10 +16090,10 @@
       <c r="E239" t="s">
         <v>324</v>
       </c>
-      <c r="H239" s="51" t="s">
+      <c r="H239" s="91" t="s">
         <v>672</v>
       </c>
-      <c r="I239" s="52"/>
+      <c r="I239" s="92"/>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" t="s">
@@ -16111,8 +16111,8 @@
       <c r="E240" t="s">
         <v>324</v>
       </c>
-      <c r="H240" s="53"/>
-      <c r="I240" s="54"/>
+      <c r="H240" s="93"/>
+      <c r="I240" s="94"/>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" t="s">
@@ -16130,8 +16130,8 @@
       <c r="E241" t="s">
         <v>324</v>
       </c>
-      <c r="H241" s="53"/>
-      <c r="I241" s="54"/>
+      <c r="H241" s="93"/>
+      <c r="I241" s="94"/>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" t="s">
@@ -16149,8 +16149,8 @@
       <c r="E242" t="s">
         <v>324</v>
       </c>
-      <c r="H242" s="53"/>
-      <c r="I242" s="54"/>
+      <c r="H242" s="93"/>
+      <c r="I242" s="94"/>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" t="s">
@@ -16168,8 +16168,8 @@
       <c r="E243" t="s">
         <v>324</v>
       </c>
-      <c r="H243" s="53"/>
-      <c r="I243" s="54"/>
+      <c r="H243" s="93"/>
+      <c r="I243" s="94"/>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" t="s">
@@ -16187,8 +16187,8 @@
       <c r="E244" t="s">
         <v>324</v>
       </c>
-      <c r="H244" s="53"/>
-      <c r="I244" s="54"/>
+      <c r="H244" s="93"/>
+      <c r="I244" s="94"/>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" t="s">
@@ -16206,8 +16206,8 @@
       <c r="E245" t="s">
         <v>324</v>
       </c>
-      <c r="H245" s="53"/>
-      <c r="I245" s="54"/>
+      <c r="H245" s="93"/>
+      <c r="I245" s="94"/>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" t="s">
@@ -16225,8 +16225,8 @@
       <c r="E246" t="s">
         <v>324</v>
       </c>
-      <c r="H246" s="53"/>
-      <c r="I246" s="54"/>
+      <c r="H246" s="93"/>
+      <c r="I246" s="94"/>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" t="s">
@@ -16244,8 +16244,8 @@
       <c r="E247" t="s">
         <v>324</v>
       </c>
-      <c r="H247" s="53"/>
-      <c r="I247" s="54"/>
+      <c r="H247" s="93"/>
+      <c r="I247" s="94"/>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" t="s">
@@ -16263,8 +16263,8 @@
       <c r="E248" t="s">
         <v>324</v>
       </c>
-      <c r="H248" s="53"/>
-      <c r="I248" s="54"/>
+      <c r="H248" s="93"/>
+      <c r="I248" s="94"/>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" t="s">
@@ -16282,8 +16282,8 @@
       <c r="E249" t="s">
         <v>324</v>
       </c>
-      <c r="H249" s="53"/>
-      <c r="I249" s="54"/>
+      <c r="H249" s="93"/>
+      <c r="I249" s="94"/>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" t="s">
@@ -16301,8 +16301,8 @@
       <c r="E250" t="s">
         <v>324</v>
       </c>
-      <c r="H250" s="53"/>
-      <c r="I250" s="54"/>
+      <c r="H250" s="93"/>
+      <c r="I250" s="94"/>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" t="s">
@@ -16320,8 +16320,8 @@
       <c r="E251" t="s">
         <v>324</v>
       </c>
-      <c r="H251" s="53"/>
-      <c r="I251" s="54"/>
+      <c r="H251" s="93"/>
+      <c r="I251" s="94"/>
     </row>
     <row r="252" spans="1:9" ht="15" thickBot="1">
       <c r="A252" t="s">
@@ -16339,8 +16339,8 @@
       <c r="E252" t="s">
         <v>324</v>
       </c>
-      <c r="H252" s="55"/>
-      <c r="I252" s="56"/>
+      <c r="H252" s="95"/>
+      <c r="I252" s="96"/>
     </row>
     <row r="253" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B253" s="38"/>
@@ -16362,10 +16362,10 @@
       <c r="E254" t="s">
         <v>324</v>
       </c>
-      <c r="H254" s="51" t="s">
+      <c r="H254" s="91" t="s">
         <v>673</v>
       </c>
-      <c r="I254" s="52"/>
+      <c r="I254" s="92"/>
     </row>
     <row r="255" spans="1:9">
       <c r="A255" t="s">
@@ -16383,8 +16383,8 @@
       <c r="E255" t="s">
         <v>324</v>
       </c>
-      <c r="H255" s="53"/>
-      <c r="I255" s="54"/>
+      <c r="H255" s="93"/>
+      <c r="I255" s="94"/>
     </row>
     <row r="256" spans="1:9">
       <c r="A256" t="s">
@@ -16402,8 +16402,8 @@
       <c r="E256" t="s">
         <v>324</v>
       </c>
-      <c r="H256" s="53"/>
-      <c r="I256" s="54"/>
+      <c r="H256" s="93"/>
+      <c r="I256" s="94"/>
     </row>
     <row r="257" spans="1:9" ht="15" thickBot="1">
       <c r="A257" t="s">
@@ -16421,8 +16421,8 @@
       <c r="E257" t="s">
         <v>324</v>
       </c>
-      <c r="H257" s="55"/>
-      <c r="I257" s="56"/>
+      <c r="H257" s="95"/>
+      <c r="I257" s="96"/>
     </row>
     <row r="258" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B258" s="38"/>
@@ -16444,10 +16444,10 @@
       <c r="E259" t="s">
         <v>324</v>
       </c>
-      <c r="H259" s="58" t="s">
+      <c r="H259" s="97" t="s">
         <v>674</v>
       </c>
-      <c r="I259" s="58"/>
+      <c r="I259" s="97"/>
     </row>
     <row r="260" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B260" s="38"/>
@@ -16469,10 +16469,10 @@
       <c r="E261" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="H261" s="51" t="s">
+      <c r="H261" s="91" t="s">
         <v>685</v>
       </c>
-      <c r="I261" s="52"/>
+      <c r="I261" s="92"/>
     </row>
     <row r="262" spans="1:9">
       <c r="A262" s="50" t="s">
@@ -16490,8 +16490,8 @@
       <c r="E262" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="H262" s="53"/>
-      <c r="I262" s="54"/>
+      <c r="H262" s="93"/>
+      <c r="I262" s="94"/>
     </row>
     <row r="263" spans="1:9">
       <c r="A263" t="s">
@@ -16509,8 +16509,8 @@
       <c r="E263" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="H263" s="53"/>
-      <c r="I263" s="54"/>
+      <c r="H263" s="93"/>
+      <c r="I263" s="94"/>
     </row>
     <row r="264" spans="1:9">
       <c r="A264" t="s">
@@ -16528,8 +16528,8 @@
       <c r="E264" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="H264" s="53"/>
-      <c r="I264" s="54"/>
+      <c r="H264" s="93"/>
+      <c r="I264" s="94"/>
     </row>
     <row r="265" spans="1:9">
       <c r="A265" t="s">
@@ -16547,8 +16547,8 @@
       <c r="E265" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="H265" s="53"/>
-      <c r="I265" s="54"/>
+      <c r="H265" s="93"/>
+      <c r="I265" s="94"/>
     </row>
     <row r="266" spans="1:9" ht="15" thickBot="1">
       <c r="A266" t="s">
@@ -16566,8 +16566,8 @@
       <c r="E266" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="H266" s="55"/>
-      <c r="I266" s="56"/>
+      <c r="H266" s="95"/>
+      <c r="I266" s="96"/>
     </row>
     <row r="267" spans="1:9" s="24" customFormat="1" ht="15" thickTop="1">
       <c r="B267" s="38"/>
@@ -17558,11 +17558,16 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H188:I194"/>
-    <mergeCell ref="H196:I199"/>
-    <mergeCell ref="H201:I206"/>
-    <mergeCell ref="H208:I212"/>
-    <mergeCell ref="H214:I223"/>
+    <mergeCell ref="H261:I266"/>
+    <mergeCell ref="H225:I237"/>
+    <mergeCell ref="H239:I252"/>
+    <mergeCell ref="H254:I257"/>
+    <mergeCell ref="H259:I259"/>
+    <mergeCell ref="H149:I158"/>
+    <mergeCell ref="H160:I166"/>
+    <mergeCell ref="H168:I170"/>
+    <mergeCell ref="H172:I179"/>
+    <mergeCell ref="H181:I186"/>
     <mergeCell ref="H3:I13"/>
     <mergeCell ref="H15:I23"/>
     <mergeCell ref="H25:I31"/>
@@ -17578,16 +17583,11 @@
     <mergeCell ref="H97:I102"/>
     <mergeCell ref="H104:I108"/>
     <mergeCell ref="H110:I119"/>
-    <mergeCell ref="H149:I158"/>
-    <mergeCell ref="H160:I166"/>
-    <mergeCell ref="H168:I170"/>
-    <mergeCell ref="H172:I179"/>
-    <mergeCell ref="H181:I186"/>
-    <mergeCell ref="H261:I266"/>
-    <mergeCell ref="H225:I237"/>
-    <mergeCell ref="H239:I252"/>
-    <mergeCell ref="H254:I257"/>
-    <mergeCell ref="H259:I259"/>
+    <mergeCell ref="H188:I194"/>
+    <mergeCell ref="H196:I199"/>
+    <mergeCell ref="H201:I206"/>
+    <mergeCell ref="H208:I212"/>
+    <mergeCell ref="H214:I223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MAP: few more sectors added
</commit_message>
<xml_diff>
--- a/new_universe.xlsx
+++ b/new_universe.xlsx
@@ -8605,58 +8605,16 @@
     <xf numFmtId="49" fontId="11" fillId="5" borderId="2" xfId="4" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="4">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="7">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="2" xfId="6">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="12" borderId="2" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="2" xfId="12">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1">
@@ -8743,7 +8701,49 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="7">
+    <xf numFmtId="49" fontId="1" fillId="12" borderId="2" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="2" xfId="12">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="2" xfId="6">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9058,7 +9058,7 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
@@ -11380,10 +11380,10 @@
       <c r="G3" t="s">
         <v>321</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="58" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="73"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A4" t="s">
@@ -11404,8 +11404,8 @@
       <c r="G4" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
     </row>
     <row r="5" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A5" t="s">
@@ -11426,8 +11426,8 @@
       <c r="G5" t="s">
         <v>321</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A6" t="s">
@@ -11448,8 +11448,8 @@
       <c r="G6" t="s">
         <v>321</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
     </row>
     <row r="7" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A7" t="s">
@@ -11470,8 +11470,8 @@
       <c r="G7" t="s">
         <v>321</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A8" t="s">
@@ -11492,8 +11492,8 @@
       <c r="G8" t="s">
         <v>321</v>
       </c>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A9" t="s">
@@ -11514,8 +11514,8 @@
       <c r="G9" t="s">
         <v>321</v>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A10" t="s">
@@ -11536,8 +11536,8 @@
       <c r="G10" t="s">
         <v>321</v>
       </c>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11" t="s">
@@ -11558,8 +11558,8 @@
       <c r="G11" t="s">
         <v>321</v>
       </c>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12" t="s">
@@ -11580,8 +11580,8 @@
       <c r="G12" t="s">
         <v>321</v>
       </c>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" t="s">
@@ -11602,8 +11602,8 @@
       <c r="G13" t="s">
         <v>321</v>
       </c>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B14" s="37"/>
@@ -11628,10 +11628,10 @@
       <c r="G15" t="s">
         <v>321</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="59" t="s">
         <v>328</v>
       </c>
-      <c r="I15" s="62"/>
+      <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A16" t="s">
@@ -11652,8 +11652,8 @@
       <c r="G16" t="s">
         <v>321</v>
       </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A17" t="s">
@@ -11674,8 +11674,8 @@
       <c r="G17" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A18" t="s">
@@ -11696,8 +11696,8 @@
       <c r="G18" t="s">
         <v>321</v>
       </c>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A19" t="s">
@@ -11718,8 +11718,8 @@
       <c r="G19" t="s">
         <v>321</v>
       </c>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A20" t="s">
@@ -11740,8 +11740,8 @@
       <c r="G20" t="s">
         <v>321</v>
       </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A21" t="s">
@@ -11762,8 +11762,8 @@
       <c r="G21" t="s">
         <v>321</v>
       </c>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A22" t="s">
@@ -11784,8 +11784,8 @@
       <c r="G22" t="s">
         <v>321</v>
       </c>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A23" t="s">
@@ -11806,8 +11806,8 @@
       <c r="G23" t="s">
         <v>321</v>
       </c>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B24" s="37"/>
@@ -11832,10 +11832,10 @@
       <c r="G25" t="s">
         <v>321</v>
       </c>
-      <c r="H25" s="74" t="s">
+      <c r="H25" s="60" t="s">
         <v>331</v>
       </c>
-      <c r="I25" s="74"/>
+      <c r="I25" s="60"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A26" t="s">
@@ -11856,8 +11856,8 @@
       <c r="G26" t="s">
         <v>321</v>
       </c>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
     </row>
     <row r="27" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A27" t="s">
@@ -11878,8 +11878,8 @@
       <c r="G27" t="s">
         <v>321</v>
       </c>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
     </row>
     <row r="28" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A28" t="s">
@@ -11900,8 +11900,8 @@
       <c r="G28" t="s">
         <v>321</v>
       </c>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
     </row>
     <row r="29" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A29" t="s">
@@ -11922,8 +11922,8 @@
       <c r="G29" t="s">
         <v>321</v>
       </c>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
     </row>
     <row r="30" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A30" t="s">
@@ -11944,8 +11944,8 @@
       <c r="G30" t="s">
         <v>321</v>
       </c>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
     </row>
     <row r="31" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A31" t="s">
@@ -11966,8 +11966,8 @@
       <c r="G31" t="s">
         <v>321</v>
       </c>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
     </row>
     <row r="32" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B32" s="37"/>
@@ -11992,10 +11992,10 @@
       <c r="G33" t="s">
         <v>321</v>
       </c>
-      <c r="H33" s="75" t="s">
+      <c r="H33" s="61" t="s">
         <v>333</v>
       </c>
-      <c r="I33" s="75"/>
+      <c r="I33" s="61"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
@@ -12016,8 +12016,8 @@
       <c r="G34" t="s">
         <v>321</v>
       </c>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
@@ -12038,8 +12038,8 @@
       <c r="G35" t="s">
         <v>321</v>
       </c>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
@@ -12060,8 +12060,8 @@
       <c r="G36" t="s">
         <v>321</v>
       </c>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
@@ -12082,8 +12082,8 @@
       <c r="G37" t="s">
         <v>321</v>
       </c>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
@@ -12104,8 +12104,8 @@
       <c r="G38" t="s">
         <v>321</v>
       </c>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
@@ -12126,8 +12126,8 @@
       <c r="G39" t="s">
         <v>321</v>
       </c>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
@@ -12148,8 +12148,8 @@
       <c r="G40" t="s">
         <v>321</v>
       </c>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
@@ -12170,8 +12170,8 @@
       <c r="G41" t="s">
         <v>321</v>
       </c>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
@@ -12192,8 +12192,8 @@
       <c r="G42" t="s">
         <v>321</v>
       </c>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
     </row>
     <row r="43" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B43" s="37"/>
@@ -12220,10 +12220,10 @@
       <c r="G44" t="s">
         <v>321</v>
       </c>
-      <c r="H44" s="74" t="s">
+      <c r="H44" s="60" t="s">
         <v>335</v>
       </c>
-      <c r="I44" s="74"/>
+      <c r="I44" s="60"/>
     </row>
     <row r="45" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A45" t="s">
@@ -12244,8 +12244,8 @@
       <c r="G45" t="s">
         <v>321</v>
       </c>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
     </row>
     <row r="46" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A46" t="s">
@@ -12266,8 +12266,8 @@
       <c r="G46" t="s">
         <v>321</v>
       </c>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
     </row>
     <row r="47" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A47" t="s">
@@ -12288,8 +12288,8 @@
       <c r="G47" t="s">
         <v>321</v>
       </c>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
     </row>
     <row r="48" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" t="s">
@@ -12310,8 +12310,8 @@
       <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="H48" s="74"/>
-      <c r="I48" s="74"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
     </row>
     <row r="49" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A49" t="s">
@@ -12332,8 +12332,8 @@
       <c r="G49" t="s">
         <v>321</v>
       </c>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
     </row>
     <row r="50" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B50" s="37"/>
@@ -12358,10 +12358,10 @@
       <c r="G51" t="s">
         <v>321</v>
       </c>
-      <c r="H51" s="84" t="s">
+      <c r="H51" s="70" t="s">
         <v>336</v>
       </c>
-      <c r="I51" s="85"/>
+      <c r="I51" s="71"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
@@ -12382,8 +12382,8 @@
       <c r="G52" t="s">
         <v>321</v>
       </c>
-      <c r="H52" s="86"/>
-      <c r="I52" s="87"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="73"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
@@ -12404,8 +12404,8 @@
       <c r="G53" t="s">
         <v>321</v>
       </c>
-      <c r="H53" s="86"/>
-      <c r="I53" s="87"/>
+      <c r="H53" s="72"/>
+      <c r="I53" s="73"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
@@ -12426,8 +12426,8 @@
       <c r="G54" t="s">
         <v>321</v>
       </c>
-      <c r="H54" s="86"/>
-      <c r="I54" s="87"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="73"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
@@ -12448,8 +12448,8 @@
       <c r="G55" t="s">
         <v>321</v>
       </c>
-      <c r="H55" s="86"/>
-      <c r="I55" s="87"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="73"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
@@ -12470,8 +12470,8 @@
       <c r="G56" t="s">
         <v>321</v>
       </c>
-      <c r="H56" s="86"/>
-      <c r="I56" s="87"/>
+      <c r="H56" s="72"/>
+      <c r="I56" s="73"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
@@ -12492,8 +12492,8 @@
       <c r="G57" t="s">
         <v>321</v>
       </c>
-      <c r="H57" s="86"/>
-      <c r="I57" s="87"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="73"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
@@ -12514,8 +12514,8 @@
       <c r="G58" t="s">
         <v>321</v>
       </c>
-      <c r="H58" s="86"/>
-      <c r="I58" s="87"/>
+      <c r="H58" s="72"/>
+      <c r="I58" s="73"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -12536,8 +12536,8 @@
       <c r="G59" t="s">
         <v>321</v>
       </c>
-      <c r="H59" s="86"/>
-      <c r="I59" s="87"/>
+      <c r="H59" s="72"/>
+      <c r="I59" s="73"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
@@ -12558,8 +12558,8 @@
       <c r="G60" t="s">
         <v>321</v>
       </c>
-      <c r="H60" s="86"/>
-      <c r="I60" s="87"/>
+      <c r="H60" s="72"/>
+      <c r="I60" s="73"/>
     </row>
     <row r="61" spans="1:9" ht="15" thickBot="1">
       <c r="A61" t="s">
@@ -12577,8 +12577,8 @@
       <c r="E61" t="s">
         <v>321</v>
       </c>
-      <c r="H61" s="88"/>
-      <c r="I61" s="89"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="75"/>
     </row>
     <row r="62" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B62" s="37"/>
@@ -12603,10 +12603,10 @@
       <c r="G63" t="s">
         <v>321</v>
       </c>
-      <c r="H63" s="62" t="s">
+      <c r="H63" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="I63" s="62"/>
+      <c r="I63" s="59"/>
     </row>
     <row r="64" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A64" t="s">
@@ -12627,8 +12627,8 @@
       <c r="G64" t="s">
         <v>321</v>
       </c>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="59"/>
     </row>
     <row r="65" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A65" t="s">
@@ -12649,8 +12649,8 @@
       <c r="G65" t="s">
         <v>321</v>
       </c>
-      <c r="H65" s="62"/>
-      <c r="I65" s="62"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
     </row>
     <row r="66" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A66" t="s">
@@ -12671,8 +12671,8 @@
       <c r="G66" t="s">
         <v>321</v>
       </c>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
     </row>
     <row r="67" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A67" t="s">
@@ -12693,8 +12693,8 @@
       <c r="G67" t="s">
         <v>321</v>
       </c>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="59"/>
     </row>
     <row r="68" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B68" s="37"/>
@@ -12719,10 +12719,10 @@
       <c r="G69" t="s">
         <v>321</v>
       </c>
-      <c r="H69" s="81" t="s">
+      <c r="H69" s="67" t="s">
         <v>360</v>
       </c>
-      <c r="I69" s="81"/>
+      <c r="I69" s="67"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
@@ -12743,8 +12743,8 @@
       <c r="G70" t="s">
         <v>321</v>
       </c>
-      <c r="H70" s="82"/>
-      <c r="I70" s="82"/>
+      <c r="H70" s="68"/>
+      <c r="I70" s="68"/>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
@@ -12765,8 +12765,8 @@
       <c r="G71" t="s">
         <v>321</v>
       </c>
-      <c r="H71" s="82"/>
-      <c r="I71" s="82"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
@@ -12787,8 +12787,8 @@
       <c r="G72" t="s">
         <v>321</v>
       </c>
-      <c r="H72" s="82"/>
-      <c r="I72" s="82"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
@@ -12809,8 +12809,8 @@
       <c r="G73" t="s">
         <v>321</v>
       </c>
-      <c r="H73" s="82"/>
-      <c r="I73" s="82"/>
+      <c r="H73" s="68"/>
+      <c r="I73" s="68"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
@@ -12831,8 +12831,8 @@
       <c r="G74" t="s">
         <v>321</v>
       </c>
-      <c r="H74" s="82"/>
-      <c r="I74" s="82"/>
+      <c r="H74" s="68"/>
+      <c r="I74" s="68"/>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
@@ -12853,8 +12853,8 @@
       <c r="G75" t="s">
         <v>321</v>
       </c>
-      <c r="H75" s="82"/>
-      <c r="I75" s="82"/>
+      <c r="H75" s="68"/>
+      <c r="I75" s="68"/>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
@@ -12875,8 +12875,8 @@
       <c r="G76" t="s">
         <v>321</v>
       </c>
-      <c r="H76" s="82"/>
-      <c r="I76" s="82"/>
+      <c r="H76" s="68"/>
+      <c r="I76" s="68"/>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
@@ -12897,8 +12897,8 @@
       <c r="G77" t="s">
         <v>321</v>
       </c>
-      <c r="H77" s="82"/>
-      <c r="I77" s="82"/>
+      <c r="H77" s="68"/>
+      <c r="I77" s="68"/>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
@@ -12919,8 +12919,8 @@
       <c r="G78" t="s">
         <v>321</v>
       </c>
-      <c r="H78" s="83"/>
-      <c r="I78" s="83"/>
+      <c r="H78" s="69"/>
+      <c r="I78" s="69"/>
     </row>
     <row r="79" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B79" s="37"/>
@@ -12945,10 +12945,10 @@
       <c r="G80" t="s">
         <v>321</v>
       </c>
-      <c r="H80" s="90" t="s">
+      <c r="H80" s="76" t="s">
         <v>403</v>
       </c>
-      <c r="I80" s="91"/>
+      <c r="I80" s="77"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
@@ -12969,8 +12969,8 @@
       <c r="G81" t="s">
         <v>321</v>
       </c>
-      <c r="H81" s="92"/>
-      <c r="I81" s="93"/>
+      <c r="H81" s="78"/>
+      <c r="I81" s="79"/>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
@@ -12991,8 +12991,8 @@
       <c r="G82" t="s">
         <v>321</v>
       </c>
-      <c r="H82" s="92"/>
-      <c r="I82" s="93"/>
+      <c r="H82" s="78"/>
+      <c r="I82" s="79"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
@@ -13013,8 +13013,8 @@
       <c r="G83" t="s">
         <v>321</v>
       </c>
-      <c r="H83" s="92"/>
-      <c r="I83" s="93"/>
+      <c r="H83" s="78"/>
+      <c r="I83" s="79"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
@@ -13035,8 +13035,8 @@
       <c r="G84" t="s">
         <v>321</v>
       </c>
-      <c r="H84" s="92"/>
-      <c r="I84" s="93"/>
+      <c r="H84" s="78"/>
+      <c r="I84" s="79"/>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
@@ -13057,8 +13057,8 @@
       <c r="G85" t="s">
         <v>321</v>
       </c>
-      <c r="H85" s="92"/>
-      <c r="I85" s="93"/>
+      <c r="H85" s="78"/>
+      <c r="I85" s="79"/>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
@@ -13079,8 +13079,8 @@
       <c r="G86" t="s">
         <v>321</v>
       </c>
-      <c r="H86" s="92"/>
-      <c r="I86" s="93"/>
+      <c r="H86" s="78"/>
+      <c r="I86" s="79"/>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
@@ -13101,8 +13101,8 @@
       <c r="G87" t="s">
         <v>321</v>
       </c>
-      <c r="H87" s="92"/>
-      <c r="I87" s="93"/>
+      <c r="H87" s="78"/>
+      <c r="I87" s="79"/>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
@@ -13123,8 +13123,8 @@
       <c r="G88" t="s">
         <v>321</v>
       </c>
-      <c r="H88" s="92"/>
-      <c r="I88" s="93"/>
+      <c r="H88" s="78"/>
+      <c r="I88" s="79"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
@@ -13145,8 +13145,8 @@
       <c r="G89" t="s">
         <v>321</v>
       </c>
-      <c r="H89" s="92"/>
-      <c r="I89" s="93"/>
+      <c r="H89" s="78"/>
+      <c r="I89" s="79"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
@@ -13167,8 +13167,8 @@
       <c r="G90" t="s">
         <v>321</v>
       </c>
-      <c r="H90" s="92"/>
-      <c r="I90" s="93"/>
+      <c r="H90" s="78"/>
+      <c r="I90" s="79"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
@@ -13189,8 +13189,8 @@
       <c r="G91" t="s">
         <v>321</v>
       </c>
-      <c r="H91" s="92"/>
-      <c r="I91" s="93"/>
+      <c r="H91" s="78"/>
+      <c r="I91" s="79"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
@@ -13211,8 +13211,8 @@
       <c r="G92" t="s">
         <v>321</v>
       </c>
-      <c r="H92" s="92"/>
-      <c r="I92" s="93"/>
+      <c r="H92" s="78"/>
+      <c r="I92" s="79"/>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
@@ -13233,8 +13233,8 @@
       <c r="G93" t="s">
         <v>321</v>
       </c>
-      <c r="H93" s="92"/>
-      <c r="I93" s="93"/>
+      <c r="H93" s="78"/>
+      <c r="I93" s="79"/>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
@@ -13255,8 +13255,8 @@
       <c r="G94" t="s">
         <v>321</v>
       </c>
-      <c r="H94" s="92"/>
-      <c r="I94" s="93"/>
+      <c r="H94" s="78"/>
+      <c r="I94" s="79"/>
     </row>
     <row r="95" spans="1:9" ht="15" thickBot="1">
       <c r="A95" t="s">
@@ -13277,8 +13277,8 @@
       <c r="G95" t="s">
         <v>321</v>
       </c>
-      <c r="H95" s="94"/>
-      <c r="I95" s="95"/>
+      <c r="H95" s="80"/>
+      <c r="I95" s="81"/>
     </row>
     <row r="96" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B96" s="37"/>
@@ -13303,10 +13303,10 @@
       <c r="G97" t="s">
         <v>321</v>
       </c>
-      <c r="H97" s="74" t="s">
+      <c r="H97" s="60" t="s">
         <v>416</v>
       </c>
-      <c r="I97" s="74"/>
+      <c r="I97" s="60"/>
     </row>
     <row r="98" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A98" t="s">
@@ -13327,8 +13327,8 @@
       <c r="G98" t="s">
         <v>321</v>
       </c>
-      <c r="H98" s="74"/>
-      <c r="I98" s="74"/>
+      <c r="H98" s="60"/>
+      <c r="I98" s="60"/>
     </row>
     <row r="99" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A99" t="s">
@@ -13349,8 +13349,8 @@
       <c r="G99" t="s">
         <v>321</v>
       </c>
-      <c r="H99" s="74"/>
-      <c r="I99" s="74"/>
+      <c r="H99" s="60"/>
+      <c r="I99" s="60"/>
     </row>
     <row r="100" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A100" t="s">
@@ -13371,8 +13371,8 @@
       <c r="G100" t="s">
         <v>321</v>
       </c>
-      <c r="H100" s="74"/>
-      <c r="I100" s="74"/>
+      <c r="H100" s="60"/>
+      <c r="I100" s="60"/>
     </row>
     <row r="101" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A101" t="s">
@@ -13393,8 +13393,8 @@
       <c r="G101" t="s">
         <v>321</v>
       </c>
-      <c r="H101" s="74"/>
-      <c r="I101" s="74"/>
+      <c r="H101" s="60"/>
+      <c r="I101" s="60"/>
     </row>
     <row r="102" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A102" t="s">
@@ -13415,8 +13415,8 @@
       <c r="G102" t="s">
         <v>321</v>
       </c>
-      <c r="H102" s="74"/>
-      <c r="I102" s="74"/>
+      <c r="H102" s="60"/>
+      <c r="I102" s="60"/>
     </row>
     <row r="103" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B103" s="37"/>
@@ -13441,10 +13441,10 @@
       <c r="G104" t="s">
         <v>321</v>
       </c>
-      <c r="H104" s="84" t="s">
+      <c r="H104" s="70" t="s">
         <v>425</v>
       </c>
-      <c r="I104" s="85"/>
+      <c r="I104" s="71"/>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
@@ -13465,8 +13465,8 @@
       <c r="G105" t="s">
         <v>321</v>
       </c>
-      <c r="H105" s="86"/>
-      <c r="I105" s="87"/>
+      <c r="H105" s="72"/>
+      <c r="I105" s="73"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
@@ -13487,8 +13487,8 @@
       <c r="G106" t="s">
         <v>321</v>
       </c>
-      <c r="H106" s="86"/>
-      <c r="I106" s="87"/>
+      <c r="H106" s="72"/>
+      <c r="I106" s="73"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
@@ -13509,8 +13509,8 @@
       <c r="G107" t="s">
         <v>321</v>
       </c>
-      <c r="H107" s="86"/>
-      <c r="I107" s="87"/>
+      <c r="H107" s="72"/>
+      <c r="I107" s="73"/>
     </row>
     <row r="108" spans="1:9" ht="15" thickBot="1">
       <c r="A108" t="s">
@@ -13531,8 +13531,8 @@
       <c r="G108" t="s">
         <v>321</v>
       </c>
-      <c r="H108" s="88"/>
-      <c r="I108" s="89"/>
+      <c r="H108" s="74"/>
+      <c r="I108" s="75"/>
     </row>
     <row r="109" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B109" s="37"/>
@@ -13557,10 +13557,10 @@
       <c r="G110" t="s">
         <v>321</v>
       </c>
-      <c r="H110" s="96" t="s">
+      <c r="H110" s="82" t="s">
         <v>445</v>
       </c>
-      <c r="I110" s="97"/>
+      <c r="I110" s="83"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
@@ -13581,8 +13581,8 @@
       <c r="G111" t="s">
         <v>321</v>
       </c>
-      <c r="H111" s="98"/>
-      <c r="I111" s="99"/>
+      <c r="H111" s="84"/>
+      <c r="I111" s="85"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
@@ -13603,8 +13603,8 @@
       <c r="G112" t="s">
         <v>321</v>
       </c>
-      <c r="H112" s="98"/>
-      <c r="I112" s="99"/>
+      <c r="H112" s="84"/>
+      <c r="I112" s="85"/>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
@@ -13625,8 +13625,8 @@
       <c r="G113" t="s">
         <v>321</v>
       </c>
-      <c r="H113" s="98"/>
-      <c r="I113" s="99"/>
+      <c r="H113" s="84"/>
+      <c r="I113" s="85"/>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
@@ -13647,8 +13647,8 @@
       <c r="G114" t="s">
         <v>321</v>
       </c>
-      <c r="H114" s="98"/>
-      <c r="I114" s="99"/>
+      <c r="H114" s="84"/>
+      <c r="I114" s="85"/>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
@@ -13669,8 +13669,8 @@
       <c r="G115" t="s">
         <v>321</v>
       </c>
-      <c r="H115" s="98"/>
-      <c r="I115" s="99"/>
+      <c r="H115" s="84"/>
+      <c r="I115" s="85"/>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
@@ -13691,8 +13691,8 @@
       <c r="G116" t="s">
         <v>321</v>
       </c>
-      <c r="H116" s="98"/>
-      <c r="I116" s="99"/>
+      <c r="H116" s="84"/>
+      <c r="I116" s="85"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
@@ -13713,8 +13713,8 @@
       <c r="G117" t="s">
         <v>321</v>
       </c>
-      <c r="H117" s="98"/>
-      <c r="I117" s="99"/>
+      <c r="H117" s="84"/>
+      <c r="I117" s="85"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
@@ -13735,8 +13735,8 @@
       <c r="G118" t="s">
         <v>321</v>
       </c>
-      <c r="H118" s="98"/>
-      <c r="I118" s="99"/>
+      <c r="H118" s="84"/>
+      <c r="I118" s="85"/>
     </row>
     <row r="119" spans="1:9" ht="15" thickBot="1">
       <c r="A119" t="s">
@@ -13757,8 +13757,8 @@
       <c r="G119" t="s">
         <v>321</v>
       </c>
-      <c r="H119" s="100"/>
-      <c r="I119" s="101"/>
+      <c r="H119" s="86"/>
+      <c r="I119" s="87"/>
     </row>
     <row r="120" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B120" s="37"/>
@@ -13783,10 +13783,10 @@
       <c r="G121" t="s">
         <v>321</v>
       </c>
-      <c r="H121" s="84" t="s">
+      <c r="H121" s="70" t="s">
         <v>460</v>
       </c>
-      <c r="I121" s="85"/>
+      <c r="I121" s="71"/>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
@@ -13807,8 +13807,8 @@
       <c r="G122" t="s">
         <v>321</v>
       </c>
-      <c r="H122" s="86"/>
-      <c r="I122" s="87"/>
+      <c r="H122" s="72"/>
+      <c r="I122" s="73"/>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
@@ -13829,8 +13829,8 @@
       <c r="G123" t="s">
         <v>321</v>
       </c>
-      <c r="H123" s="86"/>
-      <c r="I123" s="87"/>
+      <c r="H123" s="72"/>
+      <c r="I123" s="73"/>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
@@ -13851,8 +13851,8 @@
       <c r="G124" t="s">
         <v>321</v>
       </c>
-      <c r="H124" s="86"/>
-      <c r="I124" s="87"/>
+      <c r="H124" s="72"/>
+      <c r="I124" s="73"/>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
@@ -13873,8 +13873,8 @@
       <c r="G125" t="s">
         <v>321</v>
       </c>
-      <c r="H125" s="86"/>
-      <c r="I125" s="87"/>
+      <c r="H125" s="72"/>
+      <c r="I125" s="73"/>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
@@ -13895,8 +13895,8 @@
       <c r="G126" t="s">
         <v>321</v>
       </c>
-      <c r="H126" s="86"/>
-      <c r="I126" s="87"/>
+      <c r="H126" s="72"/>
+      <c r="I126" s="73"/>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
@@ -13917,8 +13917,8 @@
       <c r="G127" t="s">
         <v>321</v>
       </c>
-      <c r="H127" s="86"/>
-      <c r="I127" s="87"/>
+      <c r="H127" s="72"/>
+      <c r="I127" s="73"/>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
@@ -13939,8 +13939,8 @@
       <c r="G128" t="s">
         <v>321</v>
       </c>
-      <c r="H128" s="86"/>
-      <c r="I128" s="87"/>
+      <c r="H128" s="72"/>
+      <c r="I128" s="73"/>
     </row>
     <row r="129" spans="1:9" ht="15" thickBot="1">
       <c r="A129" t="s">
@@ -13961,8 +13961,8 @@
       <c r="G129" t="s">
         <v>321</v>
       </c>
-      <c r="H129" s="88"/>
-      <c r="I129" s="89"/>
+      <c r="H129" s="74"/>
+      <c r="I129" s="75"/>
     </row>
     <row r="130" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B130" s="37"/>
@@ -13987,10 +13987,10 @@
       <c r="G131" t="s">
         <v>321</v>
       </c>
-      <c r="H131" s="74" t="s">
+      <c r="H131" s="60" t="s">
         <v>476</v>
       </c>
-      <c r="I131" s="74"/>
+      <c r="I131" s="60"/>
     </row>
     <row r="132" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A132" t="s">
@@ -14011,8 +14011,8 @@
       <c r="G132" t="s">
         <v>321</v>
       </c>
-      <c r="H132" s="74"/>
-      <c r="I132" s="74"/>
+      <c r="H132" s="60"/>
+      <c r="I132" s="60"/>
     </row>
     <row r="133" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A133" t="s">
@@ -14033,8 +14033,8 @@
       <c r="G133" t="s">
         <v>321</v>
       </c>
-      <c r="H133" s="74"/>
-      <c r="I133" s="74"/>
+      <c r="H133" s="60"/>
+      <c r="I133" s="60"/>
     </row>
     <row r="134" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A134" t="s">
@@ -14055,8 +14055,8 @@
       <c r="G134" t="s">
         <v>321</v>
       </c>
-      <c r="H134" s="74"/>
-      <c r="I134" s="74"/>
+      <c r="H134" s="60"/>
+      <c r="I134" s="60"/>
     </row>
     <row r="135" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A135" t="s">
@@ -14077,8 +14077,8 @@
       <c r="G135" t="s">
         <v>321</v>
       </c>
-      <c r="H135" s="74"/>
-      <c r="I135" s="74"/>
+      <c r="H135" s="60"/>
+      <c r="I135" s="60"/>
     </row>
     <row r="136" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A136" t="s">
@@ -14099,8 +14099,8 @@
       <c r="G136" t="s">
         <v>321</v>
       </c>
-      <c r="H136" s="74"/>
-      <c r="I136" s="74"/>
+      <c r="H136" s="60"/>
+      <c r="I136" s="60"/>
     </row>
     <row r="137" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A137" t="s">
@@ -14121,8 +14121,8 @@
       <c r="G137" t="s">
         <v>321</v>
       </c>
-      <c r="H137" s="74"/>
-      <c r="I137" s="74"/>
+      <c r="H137" s="60"/>
+      <c r="I137" s="60"/>
     </row>
     <row r="138" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A138" t="s">
@@ -14143,8 +14143,8 @@
       <c r="G138" t="s">
         <v>321</v>
       </c>
-      <c r="H138" s="74"/>
-      <c r="I138" s="74"/>
+      <c r="H138" s="60"/>
+      <c r="I138" s="60"/>
     </row>
     <row r="139" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B139" s="37"/>
@@ -14169,10 +14169,10 @@
       <c r="G140" t="s">
         <v>321</v>
       </c>
-      <c r="H140" s="78" t="s">
+      <c r="H140" s="64" t="s">
         <v>493</v>
       </c>
-      <c r="I140" s="78"/>
+      <c r="I140" s="64"/>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" t="s">
@@ -14193,8 +14193,8 @@
       <c r="G141" t="s">
         <v>321</v>
       </c>
-      <c r="H141" s="79"/>
-      <c r="I141" s="79"/>
+      <c r="H141" s="65"/>
+      <c r="I141" s="65"/>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" t="s">
@@ -14215,8 +14215,8 @@
       <c r="G142" t="s">
         <v>321</v>
       </c>
-      <c r="H142" s="79"/>
-      <c r="I142" s="79"/>
+      <c r="H142" s="65"/>
+      <c r="I142" s="65"/>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" t="s">
@@ -14237,8 +14237,8 @@
       <c r="G143" t="s">
         <v>321</v>
       </c>
-      <c r="H143" s="79"/>
-      <c r="I143" s="79"/>
+      <c r="H143" s="65"/>
+      <c r="I143" s="65"/>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="40" t="s">
@@ -14259,8 +14259,8 @@
       <c r="G144" t="s">
         <v>321</v>
       </c>
-      <c r="H144" s="79"/>
-      <c r="I144" s="79"/>
+      <c r="H144" s="65"/>
+      <c r="I144" s="65"/>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" t="s">
@@ -14281,8 +14281,8 @@
       <c r="G145" t="s">
         <v>321</v>
       </c>
-      <c r="H145" s="79"/>
-      <c r="I145" s="79"/>
+      <c r="H145" s="65"/>
+      <c r="I145" s="65"/>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" t="s">
@@ -14303,8 +14303,8 @@
       <c r="G146" t="s">
         <v>321</v>
       </c>
-      <c r="H146" s="79"/>
-      <c r="I146" s="79"/>
+      <c r="H146" s="65"/>
+      <c r="I146" s="65"/>
     </row>
     <row r="147" spans="1:9">
       <c r="A147" t="s">
@@ -14325,8 +14325,8 @@
       <c r="G147" t="s">
         <v>321</v>
       </c>
-      <c r="H147" s="80"/>
-      <c r="I147" s="80"/>
+      <c r="H147" s="66"/>
+      <c r="I147" s="66"/>
     </row>
     <row r="148" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1">
       <c r="B148" s="37"/>
@@ -14351,10 +14351,10 @@
       <c r="G149" t="s">
         <v>321</v>
       </c>
-      <c r="H149" s="64" t="s">
+      <c r="H149" s="56" t="s">
         <v>515</v>
       </c>
-      <c r="I149" s="64"/>
+      <c r="I149" s="56"/>
     </row>
     <row r="150" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A150" t="s">
@@ -14375,8 +14375,8 @@
       <c r="G150" t="s">
         <v>321</v>
       </c>
-      <c r="H150" s="64"/>
-      <c r="I150" s="64"/>
+      <c r="H150" s="56"/>
+      <c r="I150" s="56"/>
     </row>
     <row r="151" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A151" t="s">
@@ -14397,8 +14397,8 @@
       <c r="G151" t="s">
         <v>321</v>
       </c>
-      <c r="H151" s="64"/>
-      <c r="I151" s="64"/>
+      <c r="H151" s="56"/>
+      <c r="I151" s="56"/>
     </row>
     <row r="152" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A152" t="s">
@@ -14419,8 +14419,8 @@
       <c r="G152" t="s">
         <v>321</v>
       </c>
-      <c r="H152" s="64"/>
-      <c r="I152" s="64"/>
+      <c r="H152" s="56"/>
+      <c r="I152" s="56"/>
     </row>
     <row r="153" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A153" t="s">
@@ -14441,8 +14441,8 @@
       <c r="G153" t="s">
         <v>321</v>
       </c>
-      <c r="H153" s="64"/>
-      <c r="I153" s="64"/>
+      <c r="H153" s="56"/>
+      <c r="I153" s="56"/>
     </row>
     <row r="154" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A154" t="s">
@@ -14463,8 +14463,8 @@
       <c r="G154" t="s">
         <v>321</v>
       </c>
-      <c r="H154" s="64"/>
-      <c r="I154" s="64"/>
+      <c r="H154" s="56"/>
+      <c r="I154" s="56"/>
     </row>
     <row r="155" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A155" t="s">
@@ -14485,8 +14485,8 @@
       <c r="G155" t="s">
         <v>321</v>
       </c>
-      <c r="H155" s="64"/>
-      <c r="I155" s="64"/>
+      <c r="H155" s="56"/>
+      <c r="I155" s="56"/>
     </row>
     <row r="156" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A156" t="s">
@@ -14507,8 +14507,8 @@
       <c r="G156" t="s">
         <v>321</v>
       </c>
-      <c r="H156" s="64"/>
-      <c r="I156" s="64"/>
+      <c r="H156" s="56"/>
+      <c r="I156" s="56"/>
     </row>
     <row r="157" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A157" t="s">
@@ -14529,8 +14529,8 @@
       <c r="G157" t="s">
         <v>321</v>
       </c>
-      <c r="H157" s="64"/>
-      <c r="I157" s="64"/>
+      <c r="H157" s="56"/>
+      <c r="I157" s="56"/>
     </row>
     <row r="158" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A158" t="s">
@@ -14551,8 +14551,8 @@
       <c r="G158" t="s">
         <v>321</v>
       </c>
-      <c r="H158" s="64"/>
-      <c r="I158" s="64"/>
+      <c r="H158" s="56"/>
+      <c r="I158" s="56"/>
     </row>
     <row r="159" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B159" s="37"/>
@@ -14577,10 +14577,10 @@
       <c r="G160" t="s">
         <v>321</v>
       </c>
-      <c r="H160" s="65" t="s">
+      <c r="H160" s="88" t="s">
         <v>529</v>
       </c>
-      <c r="I160" s="65"/>
+      <c r="I160" s="88"/>
     </row>
     <row r="161" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A161" t="s">
@@ -14601,8 +14601,8 @@
       <c r="G161" t="s">
         <v>321</v>
       </c>
-      <c r="H161" s="65"/>
-      <c r="I161" s="65"/>
+      <c r="H161" s="88"/>
+      <c r="I161" s="88"/>
     </row>
     <row r="162" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A162" t="s">
@@ -14623,8 +14623,8 @@
       <c r="G162" t="s">
         <v>321</v>
       </c>
-      <c r="H162" s="65"/>
-      <c r="I162" s="65"/>
+      <c r="H162" s="88"/>
+      <c r="I162" s="88"/>
     </row>
     <row r="163" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A163" t="s">
@@ -14645,8 +14645,8 @@
       <c r="G163" t="s">
         <v>321</v>
       </c>
-      <c r="H163" s="65"/>
-      <c r="I163" s="65"/>
+      <c r="H163" s="88"/>
+      <c r="I163" s="88"/>
     </row>
     <row r="164" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A164" t="s">
@@ -14667,8 +14667,8 @@
       <c r="G164" t="s">
         <v>321</v>
       </c>
-      <c r="H164" s="65"/>
-      <c r="I164" s="65"/>
+      <c r="H164" s="88"/>
+      <c r="I164" s="88"/>
     </row>
     <row r="165" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A165" t="s">
@@ -14689,8 +14689,8 @@
       <c r="G165" t="s">
         <v>321</v>
       </c>
-      <c r="H165" s="65"/>
-      <c r="I165" s="65"/>
+      <c r="H165" s="88"/>
+      <c r="I165" s="88"/>
     </row>
     <row r="166" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A166" t="s">
@@ -14711,8 +14711,8 @@
       <c r="G166" t="s">
         <v>321</v>
       </c>
-      <c r="H166" s="65"/>
-      <c r="I166" s="65"/>
+      <c r="H166" s="88"/>
+      <c r="I166" s="88"/>
     </row>
     <row r="167" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B167" s="37"/>
@@ -14737,10 +14737,10 @@
       <c r="G168" t="s">
         <v>321</v>
       </c>
-      <c r="H168" s="66" t="s">
+      <c r="H168" s="89" t="s">
         <v>537</v>
       </c>
-      <c r="I168" s="66"/>
+      <c r="I168" s="89"/>
     </row>
     <row r="169" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A169" t="s">
@@ -14761,8 +14761,8 @@
       <c r="G169" t="s">
         <v>321</v>
       </c>
-      <c r="H169" s="66"/>
-      <c r="I169" s="66"/>
+      <c r="H169" s="89"/>
+      <c r="I169" s="89"/>
     </row>
     <row r="170" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A170" t="s">
@@ -14783,8 +14783,8 @@
       <c r="G170" t="s">
         <v>321</v>
       </c>
-      <c r="H170" s="66"/>
-      <c r="I170" s="66"/>
+      <c r="H170" s="89"/>
+      <c r="I170" s="89"/>
     </row>
     <row r="171" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B171" s="37"/>
@@ -14809,10 +14809,10 @@
       <c r="G172" t="s">
         <v>321</v>
       </c>
-      <c r="H172" s="62" t="s">
+      <c r="H172" s="59" t="s">
         <v>554</v>
       </c>
-      <c r="I172" s="62"/>
+      <c r="I172" s="59"/>
     </row>
     <row r="173" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A173" t="s">
@@ -14833,8 +14833,8 @@
       <c r="G173" t="s">
         <v>321</v>
       </c>
-      <c r="H173" s="62"/>
-      <c r="I173" s="62"/>
+      <c r="H173" s="59"/>
+      <c r="I173" s="59"/>
     </row>
     <row r="174" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A174" t="s">
@@ -14855,8 +14855,8 @@
       <c r="G174" t="s">
         <v>321</v>
       </c>
-      <c r="H174" s="62"/>
-      <c r="I174" s="62"/>
+      <c r="H174" s="59"/>
+      <c r="I174" s="59"/>
     </row>
     <row r="175" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A175" t="s">
@@ -14877,8 +14877,8 @@
       <c r="G175" t="s">
         <v>321</v>
       </c>
-      <c r="H175" s="62"/>
-      <c r="I175" s="62"/>
+      <c r="H175" s="59"/>
+      <c r="I175" s="59"/>
     </row>
     <row r="176" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A176" t="s">
@@ -14899,8 +14899,8 @@
       <c r="G176" t="s">
         <v>321</v>
       </c>
-      <c r="H176" s="62"/>
-      <c r="I176" s="62"/>
+      <c r="H176" s="59"/>
+      <c r="I176" s="59"/>
     </row>
     <row r="177" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A177" t="s">
@@ -14921,8 +14921,8 @@
       <c r="G177" t="s">
         <v>321</v>
       </c>
-      <c r="H177" s="62"/>
-      <c r="I177" s="62"/>
+      <c r="H177" s="59"/>
+      <c r="I177" s="59"/>
     </row>
     <row r="178" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A178" t="s">
@@ -14943,8 +14943,8 @@
       <c r="G178" t="s">
         <v>321</v>
       </c>
-      <c r="H178" s="62"/>
-      <c r="I178" s="62"/>
+      <c r="H178" s="59"/>
+      <c r="I178" s="59"/>
     </row>
     <row r="179" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A179" s="40" t="s">
@@ -14965,8 +14965,8 @@
       <c r="G179" t="s">
         <v>321</v>
       </c>
-      <c r="H179" s="62"/>
-      <c r="I179" s="62"/>
+      <c r="H179" s="59"/>
+      <c r="I179" s="59"/>
     </row>
     <row r="180" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B180" s="37"/>
@@ -14991,10 +14991,10 @@
       <c r="G181" t="s">
         <v>321</v>
       </c>
-      <c r="H181" s="67" t="s">
+      <c r="H181" s="90" t="s">
         <v>562</v>
       </c>
-      <c r="I181" s="68"/>
+      <c r="I181" s="91"/>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" t="s">
@@ -15015,8 +15015,8 @@
       <c r="G182" t="s">
         <v>321</v>
       </c>
-      <c r="H182" s="69"/>
-      <c r="I182" s="70"/>
+      <c r="H182" s="92"/>
+      <c r="I182" s="93"/>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
@@ -15037,8 +15037,8 @@
       <c r="G183" t="s">
         <v>321</v>
       </c>
-      <c r="H183" s="69"/>
-      <c r="I183" s="70"/>
+      <c r="H183" s="92"/>
+      <c r="I183" s="93"/>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" t="s">
@@ -15059,8 +15059,8 @@
       <c r="G184" t="s">
         <v>321</v>
       </c>
-      <c r="H184" s="69"/>
-      <c r="I184" s="70"/>
+      <c r="H184" s="92"/>
+      <c r="I184" s="93"/>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" t="s">
@@ -15081,8 +15081,8 @@
       <c r="G185" t="s">
         <v>321</v>
       </c>
-      <c r="H185" s="69"/>
-      <c r="I185" s="70"/>
+      <c r="H185" s="92"/>
+      <c r="I185" s="93"/>
     </row>
     <row r="186" spans="1:9" ht="15" thickBot="1">
       <c r="A186" t="s">
@@ -15103,8 +15103,8 @@
       <c r="G186" t="s">
         <v>321</v>
       </c>
-      <c r="H186" s="71"/>
-      <c r="I186" s="72"/>
+      <c r="H186" s="94"/>
+      <c r="I186" s="95"/>
     </row>
     <row r="187" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B187" s="37"/>
@@ -15129,10 +15129,10 @@
       <c r="G188" t="s">
         <v>321</v>
       </c>
-      <c r="H188" s="64" t="s">
+      <c r="H188" s="56" t="s">
         <v>577</v>
       </c>
-      <c r="I188" s="64"/>
+      <c r="I188" s="56"/>
     </row>
     <row r="189" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A189" t="s">
@@ -15153,8 +15153,8 @@
       <c r="G189" t="s">
         <v>321</v>
       </c>
-      <c r="H189" s="64"/>
-      <c r="I189" s="64"/>
+      <c r="H189" s="56"/>
+      <c r="I189" s="56"/>
     </row>
     <row r="190" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A190" t="s">
@@ -15175,8 +15175,8 @@
       <c r="G190" t="s">
         <v>321</v>
       </c>
-      <c r="H190" s="64"/>
-      <c r="I190" s="64"/>
+      <c r="H190" s="56"/>
+      <c r="I190" s="56"/>
     </row>
     <row r="191" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A191" t="s">
@@ -15197,8 +15197,8 @@
       <c r="G191" t="s">
         <v>321</v>
       </c>
-      <c r="H191" s="64"/>
-      <c r="I191" s="64"/>
+      <c r="H191" s="56"/>
+      <c r="I191" s="56"/>
     </row>
     <row r="192" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A192" t="s">
@@ -15219,8 +15219,8 @@
       <c r="G192" t="s">
         <v>321</v>
       </c>
-      <c r="H192" s="64"/>
-      <c r="I192" s="64"/>
+      <c r="H192" s="56"/>
+      <c r="I192" s="56"/>
     </row>
     <row r="193" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A193" t="s">
@@ -15241,8 +15241,8 @@
       <c r="G193" t="s">
         <v>321</v>
       </c>
-      <c r="H193" s="64"/>
-      <c r="I193" s="64"/>
+      <c r="H193" s="56"/>
+      <c r="I193" s="56"/>
     </row>
     <row r="194" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A194" t="s">
@@ -15263,8 +15263,8 @@
       <c r="G194" t="s">
         <v>321</v>
       </c>
-      <c r="H194" s="64"/>
-      <c r="I194" s="64"/>
+      <c r="H194" s="56"/>
+      <c r="I194" s="56"/>
     </row>
     <row r="195" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B195" s="37"/>
@@ -15289,10 +15289,10 @@
       <c r="G196" t="s">
         <v>321</v>
       </c>
-      <c r="H196" s="102" t="s">
+      <c r="H196" s="57" t="s">
         <v>584</v>
       </c>
-      <c r="I196" s="102"/>
+      <c r="I196" s="57"/>
     </row>
     <row r="197" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A197" t="s">
@@ -15313,8 +15313,8 @@
       <c r="G197" t="s">
         <v>321</v>
       </c>
-      <c r="H197" s="102"/>
-      <c r="I197" s="102"/>
+      <c r="H197" s="57"/>
+      <c r="I197" s="57"/>
     </row>
     <row r="198" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A198" t="s">
@@ -15335,8 +15335,8 @@
       <c r="G198" t="s">
         <v>321</v>
       </c>
-      <c r="H198" s="102"/>
-      <c r="I198" s="102"/>
+      <c r="H198" s="57"/>
+      <c r="I198" s="57"/>
     </row>
     <row r="199" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A199" t="s">
@@ -15357,8 +15357,8 @@
       <c r="G199" t="s">
         <v>321</v>
       </c>
-      <c r="H199" s="102"/>
-      <c r="I199" s="102"/>
+      <c r="H199" s="57"/>
+      <c r="I199" s="57"/>
     </row>
     <row r="200" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B200" s="37"/>
@@ -15383,10 +15383,10 @@
       <c r="G201" t="s">
         <v>321</v>
       </c>
-      <c r="H201" s="73" t="s">
+      <c r="H201" s="58" t="s">
         <v>593</v>
       </c>
-      <c r="I201" s="73"/>
+      <c r="I201" s="58"/>
     </row>
     <row r="202" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A202" t="s">
@@ -15407,8 +15407,8 @@
       <c r="G202" t="s">
         <v>321</v>
       </c>
-      <c r="H202" s="73"/>
-      <c r="I202" s="73"/>
+      <c r="H202" s="58"/>
+      <c r="I202" s="58"/>
     </row>
     <row r="203" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A203" t="s">
@@ -15429,8 +15429,8 @@
       <c r="G203" t="s">
         <v>321</v>
       </c>
-      <c r="H203" s="73"/>
-      <c r="I203" s="73"/>
+      <c r="H203" s="58"/>
+      <c r="I203" s="58"/>
     </row>
     <row r="204" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A204" t="s">
@@ -15451,8 +15451,8 @@
       <c r="G204" t="s">
         <v>321</v>
       </c>
-      <c r="H204" s="73"/>
-      <c r="I204" s="73"/>
+      <c r="H204" s="58"/>
+      <c r="I204" s="58"/>
     </row>
     <row r="205" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A205" t="s">
@@ -15473,8 +15473,8 @@
       <c r="G205" t="s">
         <v>321</v>
       </c>
-      <c r="H205" s="73"/>
-      <c r="I205" s="73"/>
+      <c r="H205" s="58"/>
+      <c r="I205" s="58"/>
     </row>
     <row r="206" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A206" t="s">
@@ -15495,8 +15495,8 @@
       <c r="G206" t="s">
         <v>321</v>
       </c>
-      <c r="H206" s="73"/>
-      <c r="I206" s="73"/>
+      <c r="H206" s="58"/>
+      <c r="I206" s="58"/>
     </row>
     <row r="207" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B207" s="37"/>
@@ -15521,10 +15521,10 @@
       <c r="G208" t="s">
         <v>321</v>
       </c>
-      <c r="H208" s="62" t="s">
+      <c r="H208" s="59" t="s">
         <v>616</v>
       </c>
-      <c r="I208" s="62"/>
+      <c r="I208" s="59"/>
     </row>
     <row r="209" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A209" t="s">
@@ -15545,8 +15545,8 @@
       <c r="G209" t="s">
         <v>321</v>
       </c>
-      <c r="H209" s="62"/>
-      <c r="I209" s="62"/>
+      <c r="H209" s="59"/>
+      <c r="I209" s="59"/>
     </row>
     <row r="210" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A210" t="s">
@@ -15567,8 +15567,8 @@
       <c r="G210" t="s">
         <v>321</v>
       </c>
-      <c r="H210" s="62"/>
-      <c r="I210" s="62"/>
+      <c r="H210" s="59"/>
+      <c r="I210" s="59"/>
     </row>
     <row r="211" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A211" t="s">
@@ -15589,8 +15589,8 @@
       <c r="G211" t="s">
         <v>321</v>
       </c>
-      <c r="H211" s="62"/>
-      <c r="I211" s="62"/>
+      <c r="H211" s="59"/>
+      <c r="I211" s="59"/>
     </row>
     <row r="212" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A212" t="s">
@@ -15611,8 +15611,8 @@
       <c r="G212" t="s">
         <v>321</v>
       </c>
-      <c r="H212" s="62"/>
-      <c r="I212" s="62"/>
+      <c r="H212" s="59"/>
+      <c r="I212" s="59"/>
     </row>
     <row r="213" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B213" s="37"/>
@@ -15637,10 +15637,10 @@
       <c r="G214" t="s">
         <v>321</v>
       </c>
-      <c r="H214" s="74" t="s">
+      <c r="H214" s="60" t="s">
         <v>633</v>
       </c>
-      <c r="I214" s="74"/>
+      <c r="I214" s="60"/>
     </row>
     <row r="215" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A215" t="s">
@@ -15661,8 +15661,8 @@
       <c r="G215" t="s">
         <v>321</v>
       </c>
-      <c r="H215" s="74"/>
-      <c r="I215" s="74"/>
+      <c r="H215" s="60"/>
+      <c r="I215" s="60"/>
     </row>
     <row r="216" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A216" t="s">
@@ -15683,8 +15683,8 @@
       <c r="G216" t="s">
         <v>321</v>
       </c>
-      <c r="H216" s="74"/>
-      <c r="I216" s="74"/>
+      <c r="H216" s="60"/>
+      <c r="I216" s="60"/>
     </row>
     <row r="217" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A217" t="s">
@@ -15705,8 +15705,8 @@
       <c r="G217" t="s">
         <v>321</v>
       </c>
-      <c r="H217" s="74"/>
-      <c r="I217" s="74"/>
+      <c r="H217" s="60"/>
+      <c r="I217" s="60"/>
     </row>
     <row r="218" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A218" t="s">
@@ -15727,8 +15727,8 @@
       <c r="G218" t="s">
         <v>321</v>
       </c>
-      <c r="H218" s="74"/>
-      <c r="I218" s="74"/>
+      <c r="H218" s="60"/>
+      <c r="I218" s="60"/>
     </row>
     <row r="219" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A219" t="s">
@@ -15749,8 +15749,8 @@
       <c r="G219" t="s">
         <v>321</v>
       </c>
-      <c r="H219" s="74"/>
-      <c r="I219" s="74"/>
+      <c r="H219" s="60"/>
+      <c r="I219" s="60"/>
     </row>
     <row r="220" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A220" t="s">
@@ -15771,8 +15771,8 @@
       <c r="G220" t="s">
         <v>321</v>
       </c>
-      <c r="H220" s="74"/>
-      <c r="I220" s="74"/>
+      <c r="H220" s="60"/>
+      <c r="I220" s="60"/>
     </row>
     <row r="221" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A221" t="s">
@@ -15793,8 +15793,8 @@
       <c r="G221" t="s">
         <v>321</v>
       </c>
-      <c r="H221" s="74"/>
-      <c r="I221" s="74"/>
+      <c r="H221" s="60"/>
+      <c r="I221" s="60"/>
     </row>
     <row r="222" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A222" t="s">
@@ -15815,8 +15815,8 @@
       <c r="G222" t="s">
         <v>321</v>
       </c>
-      <c r="H222" s="74"/>
-      <c r="I222" s="74"/>
+      <c r="H222" s="60"/>
+      <c r="I222" s="60"/>
     </row>
     <row r="223" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A223" t="s">
@@ -15837,8 +15837,8 @@
       <c r="G223" t="s">
         <v>321</v>
       </c>
-      <c r="H223" s="74"/>
-      <c r="I223" s="74"/>
+      <c r="H223" s="60"/>
+      <c r="I223" s="60"/>
     </row>
     <row r="224" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B224" s="37"/>
@@ -15863,10 +15863,10 @@
       <c r="G225" t="s">
         <v>321</v>
       </c>
-      <c r="H225" s="62" t="s">
+      <c r="H225" s="59" t="s">
         <v>644</v>
       </c>
-      <c r="I225" s="62"/>
+      <c r="I225" s="59"/>
     </row>
     <row r="226" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A226" t="s">
@@ -15887,8 +15887,8 @@
       <c r="G226" t="s">
         <v>321</v>
       </c>
-      <c r="H226" s="62"/>
-      <c r="I226" s="62"/>
+      <c r="H226" s="59"/>
+      <c r="I226" s="59"/>
     </row>
     <row r="227" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A227" t="s">
@@ -15909,8 +15909,8 @@
       <c r="G227" t="s">
         <v>321</v>
       </c>
-      <c r="H227" s="62"/>
-      <c r="I227" s="62"/>
+      <c r="H227" s="59"/>
+      <c r="I227" s="59"/>
     </row>
     <row r="228" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A228" t="s">
@@ -15931,8 +15931,8 @@
       <c r="G228" t="s">
         <v>321</v>
       </c>
-      <c r="H228" s="62"/>
-      <c r="I228" s="62"/>
+      <c r="H228" s="59"/>
+      <c r="I228" s="59"/>
     </row>
     <row r="229" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A229" t="s">
@@ -15953,8 +15953,8 @@
       <c r="G229" t="s">
         <v>321</v>
       </c>
-      <c r="H229" s="62"/>
-      <c r="I229" s="62"/>
+      <c r="H229" s="59"/>
+      <c r="I229" s="59"/>
     </row>
     <row r="230" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A230" t="s">
@@ -15975,8 +15975,8 @@
       <c r="G230" t="s">
         <v>321</v>
       </c>
-      <c r="H230" s="62"/>
-      <c r="I230" s="62"/>
+      <c r="H230" s="59"/>
+      <c r="I230" s="59"/>
     </row>
     <row r="231" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A231" t="s">
@@ -15997,8 +15997,8 @@
       <c r="G231" t="s">
         <v>321</v>
       </c>
-      <c r="H231" s="62"/>
-      <c r="I231" s="62"/>
+      <c r="H231" s="59"/>
+      <c r="I231" s="59"/>
     </row>
     <row r="232" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A232" t="s">
@@ -16019,8 +16019,8 @@
       <c r="G232" t="s">
         <v>321</v>
       </c>
-      <c r="H232" s="62"/>
-      <c r="I232" s="62"/>
+      <c r="H232" s="59"/>
+      <c r="I232" s="59"/>
     </row>
     <row r="233" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A233" t="s">
@@ -16041,8 +16041,8 @@
       <c r="G233" t="s">
         <v>321</v>
       </c>
-      <c r="H233" s="62"/>
-      <c r="I233" s="62"/>
+      <c r="H233" s="59"/>
+      <c r="I233" s="59"/>
     </row>
     <row r="234" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A234" t="s">
@@ -16063,8 +16063,8 @@
       <c r="G234" t="s">
         <v>321</v>
       </c>
-      <c r="H234" s="62"/>
-      <c r="I234" s="62"/>
+      <c r="H234" s="59"/>
+      <c r="I234" s="59"/>
     </row>
     <row r="235" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A235" t="s">
@@ -16085,8 +16085,8 @@
       <c r="G235" t="s">
         <v>321</v>
       </c>
-      <c r="H235" s="62"/>
-      <c r="I235" s="62"/>
+      <c r="H235" s="59"/>
+      <c r="I235" s="59"/>
     </row>
     <row r="236" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A236" t="s">
@@ -16107,8 +16107,8 @@
       <c r="G236" t="s">
         <v>321</v>
       </c>
-      <c r="H236" s="62"/>
-      <c r="I236" s="62"/>
+      <c r="H236" s="59"/>
+      <c r="I236" s="59"/>
     </row>
     <row r="237" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
       <c r="A237" t="s">
@@ -16129,8 +16129,8 @@
       <c r="G237" t="s">
         <v>321</v>
       </c>
-      <c r="H237" s="62"/>
-      <c r="I237" s="62"/>
+      <c r="H237" s="59"/>
+      <c r="I237" s="59"/>
     </row>
     <row r="238" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B238" s="37"/>
@@ -16152,10 +16152,10 @@
       <c r="E239" t="s">
         <v>321</v>
       </c>
-      <c r="H239" s="56" t="s">
+      <c r="H239" s="96" t="s">
         <v>669</v>
       </c>
-      <c r="I239" s="57"/>
+      <c r="I239" s="97"/>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" t="s">
@@ -16173,8 +16173,8 @@
       <c r="E240" t="s">
         <v>321</v>
       </c>
-      <c r="H240" s="58"/>
-      <c r="I240" s="59"/>
+      <c r="H240" s="98"/>
+      <c r="I240" s="99"/>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" t="s">
@@ -16192,8 +16192,8 @@
       <c r="E241" t="s">
         <v>321</v>
       </c>
-      <c r="H241" s="58"/>
-      <c r="I241" s="59"/>
+      <c r="H241" s="98"/>
+      <c r="I241" s="99"/>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" t="s">
@@ -16211,8 +16211,8 @@
       <c r="E242" t="s">
         <v>321</v>
       </c>
-      <c r="H242" s="58"/>
-      <c r="I242" s="59"/>
+      <c r="H242" s="98"/>
+      <c r="I242" s="99"/>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" t="s">
@@ -16230,8 +16230,8 @@
       <c r="E243" t="s">
         <v>321</v>
       </c>
-      <c r="H243" s="58"/>
-      <c r="I243" s="59"/>
+      <c r="H243" s="98"/>
+      <c r="I243" s="99"/>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" t="s">
@@ -16249,8 +16249,8 @@
       <c r="E244" t="s">
         <v>321</v>
       </c>
-      <c r="H244" s="58"/>
-      <c r="I244" s="59"/>
+      <c r="H244" s="98"/>
+      <c r="I244" s="99"/>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" t="s">
@@ -16268,8 +16268,8 @@
       <c r="E245" t="s">
         <v>321</v>
       </c>
-      <c r="H245" s="58"/>
-      <c r="I245" s="59"/>
+      <c r="H245" s="98"/>
+      <c r="I245" s="99"/>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" t="s">
@@ -16287,8 +16287,8 @@
       <c r="E246" t="s">
         <v>321</v>
       </c>
-      <c r="H246" s="58"/>
-      <c r="I246" s="59"/>
+      <c r="H246" s="98"/>
+      <c r="I246" s="99"/>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" t="s">
@@ -16306,8 +16306,8 @@
       <c r="E247" t="s">
         <v>321</v>
       </c>
-      <c r="H247" s="58"/>
-      <c r="I247" s="59"/>
+      <c r="H247" s="98"/>
+      <c r="I247" s="99"/>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" t="s">
@@ -16325,8 +16325,8 @@
       <c r="E248" t="s">
         <v>321</v>
       </c>
-      <c r="H248" s="58"/>
-      <c r="I248" s="59"/>
+      <c r="H248" s="98"/>
+      <c r="I248" s="99"/>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" t="s">
@@ -16344,8 +16344,8 @@
       <c r="E249" t="s">
         <v>321</v>
       </c>
-      <c r="H249" s="58"/>
-      <c r="I249" s="59"/>
+      <c r="H249" s="98"/>
+      <c r="I249" s="99"/>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" t="s">
@@ -16363,8 +16363,8 @@
       <c r="E250" t="s">
         <v>321</v>
       </c>
-      <c r="H250" s="58"/>
-      <c r="I250" s="59"/>
+      <c r="H250" s="98"/>
+      <c r="I250" s="99"/>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" t="s">
@@ -16382,8 +16382,8 @@
       <c r="E251" t="s">
         <v>321</v>
       </c>
-      <c r="H251" s="58"/>
-      <c r="I251" s="59"/>
+      <c r="H251" s="98"/>
+      <c r="I251" s="99"/>
     </row>
     <row r="252" spans="1:9" ht="15" thickBot="1">
       <c r="A252" t="s">
@@ -16401,8 +16401,8 @@
       <c r="E252" t="s">
         <v>321</v>
       </c>
-      <c r="H252" s="60"/>
-      <c r="I252" s="61"/>
+      <c r="H252" s="100"/>
+      <c r="I252" s="101"/>
     </row>
     <row r="253" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B253" s="37"/>
@@ -16424,10 +16424,10 @@
       <c r="E254" t="s">
         <v>321</v>
       </c>
-      <c r="H254" s="56" t="s">
+      <c r="H254" s="96" t="s">
         <v>670</v>
       </c>
-      <c r="I254" s="57"/>
+      <c r="I254" s="97"/>
     </row>
     <row r="255" spans="1:9">
       <c r="A255" t="s">
@@ -16445,8 +16445,8 @@
       <c r="E255" t="s">
         <v>321</v>
       </c>
-      <c r="H255" s="58"/>
-      <c r="I255" s="59"/>
+      <c r="H255" s="98"/>
+      <c r="I255" s="99"/>
     </row>
     <row r="256" spans="1:9">
       <c r="A256" t="s">
@@ -16464,8 +16464,8 @@
       <c r="E256" t="s">
         <v>321</v>
       </c>
-      <c r="H256" s="58"/>
-      <c r="I256" s="59"/>
+      <c r="H256" s="98"/>
+      <c r="I256" s="99"/>
     </row>
     <row r="257" spans="1:9" ht="15" thickBot="1">
       <c r="A257" t="s">
@@ -16483,8 +16483,8 @@
       <c r="E257" t="s">
         <v>321</v>
       </c>
-      <c r="H257" s="60"/>
-      <c r="I257" s="61"/>
+      <c r="H257" s="100"/>
+      <c r="I257" s="101"/>
     </row>
     <row r="258" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B258" s="37"/>
@@ -16506,10 +16506,10 @@
       <c r="E259" t="s">
         <v>321</v>
       </c>
-      <c r="H259" s="63" t="s">
+      <c r="H259" s="102" t="s">
         <v>671</v>
       </c>
-      <c r="I259" s="63"/>
+      <c r="I259" s="102"/>
     </row>
     <row r="260" spans="1:9" s="24" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="B260" s="37"/>
@@ -16531,10 +16531,10 @@
       <c r="E261" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="H261" s="56" t="s">
+      <c r="H261" s="96" t="s">
         <v>682</v>
       </c>
-      <c r="I261" s="57"/>
+      <c r="I261" s="97"/>
     </row>
     <row r="262" spans="1:9">
       <c r="A262" s="47" t="s">
@@ -16552,8 +16552,8 @@
       <c r="E262" s="47" t="s">
         <v>321</v>
       </c>
-      <c r="H262" s="58"/>
-      <c r="I262" s="59"/>
+      <c r="H262" s="98"/>
+      <c r="I262" s="99"/>
     </row>
     <row r="263" spans="1:9">
       <c r="A263" t="s">
@@ -16571,8 +16571,8 @@
       <c r="E263" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="H263" s="58"/>
-      <c r="I263" s="59"/>
+      <c r="H263" s="98"/>
+      <c r="I263" s="99"/>
     </row>
     <row r="264" spans="1:9">
       <c r="A264" t="s">
@@ -16590,8 +16590,8 @@
       <c r="E264" s="47" t="s">
         <v>321</v>
       </c>
-      <c r="H264" s="58"/>
-      <c r="I264" s="59"/>
+      <c r="H264" s="98"/>
+      <c r="I264" s="99"/>
     </row>
     <row r="265" spans="1:9">
       <c r="A265" t="s">
@@ -16609,8 +16609,8 @@
       <c r="E265" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="H265" s="58"/>
-      <c r="I265" s="59"/>
+      <c r="H265" s="98"/>
+      <c r="I265" s="99"/>
     </row>
     <row r="266" spans="1:9" ht="15" thickBot="1">
       <c r="A266" t="s">
@@ -16628,8 +16628,8 @@
       <c r="E266" s="47" t="s">
         <v>321</v>
       </c>
-      <c r="H266" s="60"/>
-      <c r="I266" s="61"/>
+      <c r="H266" s="100"/>
+      <c r="I266" s="101"/>
     </row>
     <row r="267" spans="1:9" s="24" customFormat="1" ht="15" thickTop="1">
       <c r="B267" s="37"/>
@@ -17620,11 +17620,16 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H188:I194"/>
-    <mergeCell ref="H196:I199"/>
-    <mergeCell ref="H201:I206"/>
-    <mergeCell ref="H208:I212"/>
-    <mergeCell ref="H214:I223"/>
+    <mergeCell ref="H261:I266"/>
+    <mergeCell ref="H225:I237"/>
+    <mergeCell ref="H239:I252"/>
+    <mergeCell ref="H254:I257"/>
+    <mergeCell ref="H259:I259"/>
+    <mergeCell ref="H149:I158"/>
+    <mergeCell ref="H160:I166"/>
+    <mergeCell ref="H168:I170"/>
+    <mergeCell ref="H172:I179"/>
+    <mergeCell ref="H181:I186"/>
     <mergeCell ref="H3:I13"/>
     <mergeCell ref="H15:I23"/>
     <mergeCell ref="H25:I31"/>
@@ -17640,16 +17645,11 @@
     <mergeCell ref="H97:I102"/>
     <mergeCell ref="H104:I108"/>
     <mergeCell ref="H110:I119"/>
-    <mergeCell ref="H149:I158"/>
-    <mergeCell ref="H160:I166"/>
-    <mergeCell ref="H168:I170"/>
-    <mergeCell ref="H172:I179"/>
-    <mergeCell ref="H181:I186"/>
-    <mergeCell ref="H261:I266"/>
-    <mergeCell ref="H225:I237"/>
-    <mergeCell ref="H239:I252"/>
-    <mergeCell ref="H254:I257"/>
-    <mergeCell ref="H259:I259"/>
+    <mergeCell ref="H188:I194"/>
+    <mergeCell ref="H196:I199"/>
+    <mergeCell ref="H201:I206"/>
+    <mergeCell ref="H208:I212"/>
+    <mergeCell ref="H214:I223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>